<commit_message>
Update condo desk review spreadsheet for 2024 model
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1B8C9F-CFDC-4BB7-B358-9CE8810B592B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25485"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
-    <sheet name="Building (PIN10)" sheetId="4" r:id="rId2"/>
+    <sheet name="Buildings" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,12 +37,36 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane</author>
+  </authors>
+  <commentList>
+    <comment ref="AA6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
+If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Daniel F. Snow</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>PIN</t>
   </si>
@@ -128,9 +155,6 @@
     <t>Land Value Capped</t>
   </si>
   <si>
-    <t>Value Unchanged</t>
-  </si>
-  <si>
     <t>YoY Change &gt;= 50%</t>
   </si>
   <si>
@@ -204,19 +228,52 @@
   </si>
   <si>
     <t>Aggregated stats by building (PIN10)</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 1</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 2</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>Land Val. &gt;= 95th Percentile</t>
+  </si>
+  <si>
+    <t>Building Val. &gt;= 95th Percentile</t>
+  </si>
+  <si>
+    <t>Initial to Final Value Changed</t>
+  </si>
+  <si>
+    <t>Prior Year Value Unchanged</t>
+  </si>
+  <si>
+    <t>PIN Information</t>
+  </si>
+  <si>
+    <t>Change In Value</t>
+  </si>
+  <si>
+    <t>Sales Information</t>
+  </si>
+  <si>
+    <t>Flags</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,8 +317,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +348,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CCFC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +479,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -396,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -406,23 +501,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -434,16 +525,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -453,6 +541,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,6 +588,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9CCFC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -771,8 +900,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA1048575"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -794,7 +923,7 @@
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
     <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
     <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
     <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
     <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
@@ -804,29 +933,34 @@
     <col min="24" max="24" width="11" style="11"/>
     <col min="25" max="25" width="10.375" customWidth="1"/>
     <col min="26" max="26" width="13" style="10" customWidth="1"/>
-    <col min="27" max="28" width="13" style="18" customWidth="1"/>
-    <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="13" style="18" customWidth="1"/>
-    <col min="34" max="34" width="11" style="13"/>
-    <col min="36" max="36" width="15.625" customWidth="1"/>
-    <col min="37" max="37" width="17.375" customWidth="1"/>
-    <col min="38" max="39" width="15.625" customWidth="1"/>
-    <col min="40" max="40" width="12.625" customWidth="1"/>
-    <col min="42" max="42" width="14" customWidth="1"/>
-    <col min="43" max="43" width="11.875" customWidth="1"/>
-    <col min="44" max="44" width="10.875" customWidth="1"/>
+    <col min="27" max="27" width="18.625" style="10" customWidth="1"/>
+    <col min="28" max="29" width="13" style="16" customWidth="1"/>
+    <col min="30" max="30" width="13" style="10" customWidth="1"/>
+    <col min="31" max="31" width="18.625" style="10" customWidth="1"/>
+    <col min="32" max="32" width="13" style="16" customWidth="1"/>
+    <col min="36" max="36" width="11" style="13"/>
+    <col min="38" max="38" width="15.625" customWidth="1"/>
+    <col min="39" max="39" width="17.375" customWidth="1"/>
+    <col min="40" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="12.625" customWidth="1"/>
+    <col min="43" max="43" width="13.25" customWidth="1"/>
+    <col min="44" max="44" width="14.125" customWidth="1"/>
+    <col min="46" max="46" width="14" customWidth="1"/>
+    <col min="47" max="47" width="14.875" customWidth="1"/>
+    <col min="48" max="48" width="11.875" customWidth="1"/>
+    <col min="49" max="49" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -871,8 +1005,13 @@
       <c r="AY1" s="5"/>
       <c r="AZ1" s="5"/>
       <c r="BA1" s="5"/>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -902,15 +1041,17 @@
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
-      <c r="AH2"/>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AJ2"/>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -935,9 +1076,11 @@
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
-      <c r="AH3"/>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AJ3"/>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -961,44 +1104,71 @@
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
-      <c r="AH4"/>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="H5"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="29"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AH5"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="26"/>
-      <c r="AQ5" s="26"/>
-      <c r="AR5" s="26"/>
-    </row>
-    <row r="6" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AJ4"/>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="31"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH5" s="32"/>
+      <c r="AI5" s="32"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL5" s="38"/>
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="38"/>
+      <c r="AO5" s="38"/>
+      <c r="AP5" s="38"/>
+      <c r="AQ5" s="38"/>
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
+      <c r="AU5" s="38"/>
+      <c r="AV5" s="38"/>
+      <c r="AW5" s="38"/>
+    </row>
+    <row r="6" spans="1:58" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>9</v>
@@ -1015,28 +1185,28 @@
         <v>10</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>37</v>
+      <c r="H6" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>8</v>
@@ -1044,11 +1214,11 @@
       <c r="O6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>5</v>
@@ -1060,7 +1230,7 @@
         <v>14</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>6</v>
@@ -1074,257 +1244,277 @@
       <c r="Y6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="Z6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AA6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AC6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="AD6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AE6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI6" s="9" t="s">
+      <c r="AM6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AJ6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AM6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN6" s="8" t="s">
+      <c r="AP6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AQ6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AR6" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="1048519" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048575" s="13"/>
+    </row>
+    <row r="1048519" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="34:34" x14ac:dyDescent="0.25">
+      <c r="AH1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
-    <mergeCell ref="AI5:AR5"/>
+    <mergeCell ref="AK5:AW5"/>
     <mergeCell ref="O5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:AF5"/>
+    <mergeCell ref="AG5:AJ5"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1343,14 +1533,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1364,17 +1554,31 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3"/>
-      <c r="K3"/>
+      <c r="B3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="33"/>
+      <c r="L3" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
@@ -1383,19 +1587,19 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -1404,10 +1608,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
@@ -1582,8 +1786,11 @@
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Get condo desk review spreadsheet working with 2023 data
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1B8C9F-CFDC-4BB7-B358-9CE8810B592B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6194AA02-3497-4A49-BDAC-44FCA267AA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>PIN</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>Land Val. &gt;= 95th Percentile</t>
-  </si>
-  <si>
-    <t>Building Val. &gt;= 95th Percentile</t>
-  </si>
-  <si>
-    <t>Initial to Final Value Changed</t>
   </si>
   <si>
     <t>Prior Year Value Unchanged</t>
@@ -479,7 +473,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -519,6 +513,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -543,40 +538,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -907,7 +908,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -915,8 +916,9 @@
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="6" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="39.125" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="15.375" customWidth="1"/>
     <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
     <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
@@ -953,14 +955,14 @@
   <sheetData>
     <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1049,9 +1051,9 @@
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1109,35 +1111,35 @@
       <c r="AJ4"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="30" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="X5" s="30"/>
-      <c r="Y5" s="36" t="s">
-        <v>57</v>
       </c>
       <c r="Z5" s="31"/>
       <c r="AA5" s="31"/>
@@ -1145,30 +1147,30 @@
       <c r="AC5" s="31"/>
       <c r="AD5" s="31"/>
       <c r="AE5" s="31"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="34" t="s">
+      <c r="AF5" s="32"/>
+      <c r="AG5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AH5" s="32"/>
-      <c r="AI5" s="32"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="34"/>
       <c r="AJ5" s="35"/>
       <c r="AK5" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL5" s="38"/>
-      <c r="AM5" s="38"/>
-      <c r="AN5" s="38"/>
-      <c r="AO5" s="38"/>
-      <c r="AP5" s="38"/>
-      <c r="AQ5" s="38"/>
-      <c r="AR5" s="38"/>
-      <c r="AS5" s="38"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="38"/>
-      <c r="AV5" s="38"/>
-      <c r="AW5" s="38"/>
-    </row>
-    <row r="6" spans="1:58" ht="31.5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="AL5" s="39"/>
+      <c r="AM5" s="39"/>
+      <c r="AN5" s="39"/>
+      <c r="AO5" s="39"/>
+      <c r="AP5" s="39"/>
+      <c r="AQ5" s="39"/>
+      <c r="AR5" s="39"/>
+      <c r="AS5" s="39"/>
+      <c r="AT5" s="39"/>
+      <c r="AU5" s="40"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
+    </row>
+    <row r="6" spans="1:58" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1292,28 +1294,22 @@
       <c r="AO6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AP6" s="8" t="s">
+      <c r="AP6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="AQ6" s="9" t="s">
         <v>51</v>
       </c>
       <c r="AR6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AS6" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="AT6" s="9" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="AU6" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AW6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1490,15 +1486,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="Y5:AF5"/>
+    <mergeCell ref="AG5:AJ5"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="AK5:AU5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
-    <mergeCell ref="AK5:AW5"/>
     <mergeCell ref="O5:V5"/>
     <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:AF5"/>
-    <mergeCell ref="AG5:AJ5"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1533,14 +1529,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1554,21 +1550,21 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="B3" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="17"/>
       <c r="I3" s="18"/>
-      <c r="J3" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34" t="s">
+      <c r="J3" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="41"/>
+      <c r="L3" s="33" t="s">
         <v>50</v>
       </c>
       <c r="M3" s="35"/>

</xml_diff>

<commit_message>
Push final res model desk review tweaks to condo model
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -2,21 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6194AA02-3497-4A49-BDAC-44FCA267AA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4A2B78-894B-42F1-BC9E-24AD988F135B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
     <sheet name="Buildings" sheetId="4" r:id="rId2"/>
+    <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AX$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,17 +49,151 @@
     <author>Jean Cochrane</author>
   </authors>
   <commentList>
-    <comment ref="AA6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
+    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
 If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates this unit is a parking space, common area, storage area, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Number of sales in the building containing this PIN in the past five years.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates this condo may be a common area (based on prior year value).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates the different shares of ownership in this condo's building do not sum to 1, meaning shares may be incorrect or incomplete.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates this condo's building spans multiple land lines.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates this condo's land value is greater than the 95th percentile of land values for its town (that is to say, it's very high).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the land value for this PIN was artificially capped below its $/sqft rate in order to remain less than 50% of the total FMV.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the PIN's value has not changed since last year, which should be unlikely.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the estimated value for the PIN is dramatically higher than last year's value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates the estimated value for the PIN is dramatically lower than last year's value.
+</t>
         </r>
       </text>
     </comment>
@@ -84,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>PIN</t>
   </si>
@@ -239,12 +380,6 @@
     <t>Characteristics</t>
   </si>
   <si>
-    <t>Land Val. &gt;= 95th Percentile</t>
-  </si>
-  <si>
-    <t>Prior Year Value Unchanged</t>
-  </si>
-  <si>
     <t>PIN Information</t>
   </si>
   <si>
@@ -255,19 +390,68 @@
   </si>
   <si>
     <t>Flags</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Valuations Notes</t>
+  </si>
+  <si>
+    <t>Lnd. &gt;= 95% in Town</t>
+  </si>
+  <si>
+    <t>Value Unchanged</t>
+  </si>
+  <si>
+    <t>Summary statistics broken out by neighborhood</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Class</t>
+  </si>
+  <si>
+    <t>Total AV</t>
+  </si>
+  <si>
+    <t>AV Difference</t>
+  </si>
+  <si>
+    <t>Min of Total AV</t>
+  </si>
+  <si>
+    <t>Average of Total AV</t>
+  </si>
+  <si>
+    <t>Max of Total AV</t>
+  </si>
+  <si>
+    <t>Average of AV Difference</t>
+  </si>
+  <si>
+    <t>Average of YoY ∆ %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,12 +496,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="0"/>
@@ -326,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,8 +547,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -466,6 +650,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -473,7 +672,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,7 +712,55 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -544,40 +791,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,6 +809,7 @@
   <colors>
     <mruColors>
       <color rgb="FFF9CCFC"/>
+      <color rgb="FFFFD1D1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -603,6 +821,355 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.611203819448" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="pin_detail_range"/>
+  </cacheSource>
+  <cacheFields count="50">
+    <cacheField name="PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Class" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nbhd." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Street Address" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Municipality" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Building ID (PIN10)" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback Key PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback Percent Ownership" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Unit Rate   S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Total" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Before Rounding" numFmtId="44">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate Original" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate     Effective" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Unit Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Tot." numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ $" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ %" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Valuations Notes" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Year Built" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total        Bld. S. F." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stories" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. S. F." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Unit S. F." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Non-Livable Space" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Bld. # Sales (Past 5 Years)" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Potential Common Area" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="% Ownership Sum Not Equal to 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Multi-Land" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. &gt;= 95% in Town" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land Value Capped" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Value Unchanged" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &gt;= 50%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total AV" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="AV Difference" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="50">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="3"/>
+    <dataField name="Min of Total AV" fld="48" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="48" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="48" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -902,13 +1469,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF1048575"/>
+  <dimension ref="A1:BG1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -916,7 +1483,7 @@
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="39.125" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
     <col min="5" max="5" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="15.375" customWidth="1"/>
@@ -933,36 +1500,37 @@
     <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="24" width="11" style="11"/>
-    <col min="25" max="25" width="10.375" customWidth="1"/>
-    <col min="26" max="26" width="13" style="10" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="10" customWidth="1"/>
-    <col min="28" max="29" width="13" style="16" customWidth="1"/>
-    <col min="30" max="30" width="13" style="10" customWidth="1"/>
-    <col min="31" max="31" width="18.625" style="10" customWidth="1"/>
-    <col min="32" max="32" width="13" style="16" customWidth="1"/>
-    <col min="36" max="36" width="11" style="13"/>
-    <col min="38" max="38" width="15.625" customWidth="1"/>
-    <col min="39" max="39" width="17.375" customWidth="1"/>
-    <col min="40" max="41" width="15.625" customWidth="1"/>
-    <col min="42" max="42" width="12.625" customWidth="1"/>
-    <col min="43" max="43" width="13.25" customWidth="1"/>
-    <col min="44" max="44" width="14.125" customWidth="1"/>
-    <col min="46" max="46" width="14" customWidth="1"/>
-    <col min="47" max="47" width="14.875" customWidth="1"/>
-    <col min="48" max="48" width="11.875" customWidth="1"/>
-    <col min="49" max="49" width="10.875" customWidth="1"/>
+    <col min="25" max="25" width="21.125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="13" customWidth="1"/>
+    <col min="27" max="27" width="13" style="10" customWidth="1"/>
+    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="30" width="13" style="16" customWidth="1"/>
+    <col min="31" max="31" width="13" style="10" customWidth="1"/>
+    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
+    <col min="33" max="33" width="13" style="16" customWidth="1"/>
+    <col min="37" max="37" width="11" style="13"/>
+    <col min="39" max="39" width="15.625" customWidth="1"/>
+    <col min="40" max="40" width="17.375" customWidth="1"/>
+    <col min="41" max="42" width="15.625" customWidth="1"/>
+    <col min="43" max="43" width="12.625" customWidth="1"/>
+    <col min="44" max="44" width="13.25" customWidth="1"/>
+    <col min="45" max="45" width="14.125" customWidth="1"/>
+    <col min="47" max="47" width="14" customWidth="1"/>
+    <col min="48" max="48" width="14.875" customWidth="1"/>
+    <col min="49" max="49" width="11.875" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1012,8 +1580,9 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1038,22 +1607,23 @@
       <c r="V2"/>
       <c r="W2"/>
       <c r="X2"/>
-      <c r="Z2"/>
+      <c r="Y2"/>
       <c r="AA2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2"/>
-      <c r="AJ2"/>
-    </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AG2"/>
+      <c r="AK2"/>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1073,16 +1643,17 @@
       <c r="V3"/>
       <c r="W3"/>
       <c r="X3"/>
-      <c r="Z3"/>
+      <c r="Y3"/>
       <c r="AA3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AF3"/>
-      <c r="AJ3"/>
-    </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AG3"/>
+      <c r="AK3"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1101,18 +1672,19 @@
       <c r="V4"/>
       <c r="W4"/>
       <c r="X4"/>
-      <c r="Z4"/>
+      <c r="Y4"/>
       <c r="AA4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4"/>
       <c r="AF4"/>
-      <c r="AJ4"/>
-    </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="AG4"/>
+      <c r="AK4"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -1120,57 +1692,60 @@
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
       <c r="H5" s="37"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="28" t="s">
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="31"/>
-      <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="32"/>
-      <c r="AG5" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL5" s="39"/>
-      <c r="AM5" s="39"/>
-      <c r="AN5" s="39"/>
-      <c r="AO5" s="39"/>
-      <c r="AP5" s="39"/>
-      <c r="AQ5" s="39"/>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="19"/>
+      <c r="AN5" s="30"/>
+      <c r="AO5" s="30"/>
+      <c r="AP5" s="30"/>
+      <c r="AQ5" s="30"/>
+      <c r="AR5" s="30"/>
+      <c r="AS5" s="30"/>
+      <c r="AT5" s="30"/>
+      <c r="AU5" s="30"/>
+      <c r="AV5" s="31"/>
       <c r="AW5" s="19"/>
-    </row>
-    <row r="6" spans="1:58" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="AX5" s="19"/>
+    </row>
+    <row r="6" spans="1:59" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1243,253 +1818,262 @@
       <c r="X6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="AA6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AB6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AC6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AD6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AE6" s="4" t="s">
+      <c r="AF6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AH6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AI6" s="3" t="s">
+      <c r="AJ6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AJ6" s="4" t="s">
+      <c r="AK6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AK6" s="9" t="s">
+      <c r="AL6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AL6" s="9" t="s">
+      <c r="AM6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AM6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AP6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AQ6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AQ6" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="AR6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AS6" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="AT6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="1048519" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="34:34" x14ac:dyDescent="0.25">
-      <c r="AH1048575" s="13"/>
+      <c r="AW6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="Y5:AF5"/>
-    <mergeCell ref="AG5:AJ5"/>
+    <mergeCell ref="AH5:AL5"/>
+    <mergeCell ref="AM5:AV5"/>
+    <mergeCell ref="Z5:AG5"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="AK5:AU5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
@@ -1510,15 +2094,15 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="5" max="6" width="11.625" customWidth="1"/>
     <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
@@ -1529,14 +2113,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1550,8 +2134,8 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
-        <v>53</v>
+      <c r="B3" s="49" t="s">
+        <v>51</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -1560,14 +2144,14 @@
       <c r="G3" s="37"/>
       <c r="H3" s="17"/>
       <c r="I3" s="18"/>
-      <c r="J3" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="33" t="s">
+      <c r="J3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="48"/>
+      <c r="L3" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="35"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1792,4 +2376,97 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4264-9F60-48E3-A5EA-D04C0BA089E2}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tweak note for land S.F. flag in desk review workbook
The previous iteration of the note was not quite correct, implying that the flag had to do with the 95th percentile of land _value_ instead of land _square footage_.
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4A2B78-894B-42F1-BC9E-24AD988F135B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2366FE96-8444-474B-9653-F87BFABDD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="14" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -140,7 +140,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates this condo's land value is greater than the 95th percentile of land values for its town (that is to say, it's very high).</t>
+          <t>Indicates this condo's land square footage is greater than the 95th percentile of land S. F. for its town (that is to say, it's very high).</t>
         </r>
       </text>
     </comment>
@@ -824,7 +824,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45331.611203819448" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.444692708334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1050,7 +1050,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="50">
     <pivotField showAll="0"/>

</xml_diff>

<commit_message>
Update desk review workbook for 2024 model (#23)
* Update condo desk review spreadsheet for 2024 model

* Get condo desk review spreadsheet working with 2023 data

* Update iasWorld output for 2024 in export pipeline stage

* Add conditional formatting to YoY % change column in desk review workbook

* Push final res model desk review tweaks to condo model

* Tweak note for land S.F. flag in desk review workbook

The previous iteration of the note was not quite correct, implying that the flag had to do with the 95th percentile of land _value_ instead of land _square footage_.

---------

Co-authored-by: William Ridgeway <10358980+wrridgeway@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2366FE96-8444-474B-9653-F87BFABDD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25485"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
-    <sheet name="Building (PIN10)" sheetId="4" r:id="rId2"/>
+    <sheet name="Buildings" sheetId="4" r:id="rId2"/>
+    <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AX$7</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="14" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,12 +44,170 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean Cochrane</author>
+  </authors>
+  <commentList>
+    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
+If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates this unit is a parking space, common area, storage area, etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Number of sales in the building containing this PIN in the past five years.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates this condo may be a common area (based on prior year value).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates the different shares of ownership in this condo's building do not sum to 1, meaning shares may be incorrect or incomplete.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates this condo's building spans multiple land lines.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates this condo's land square footage is greater than the 95th percentile of land S. F. for its town (that is to say, it's very high).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the land value for this PIN was artificially capped below its $/sqft rate in order to remain less than 50% of the total FMV.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the PIN's value has not changed since last year, which should be unlikely.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates the estimated value for the PIN is dramatically higher than last year's value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicates the estimated value for the PIN is dramatically lower than last year's value.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Daniel F. Snow</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>PIN</t>
   </si>
@@ -128,95 +296,162 @@
     <t>Land Value Capped</t>
   </si>
   <si>
+    <t>YoY Change &gt;= 50%</t>
+  </si>
+  <si>
+    <t>YoY Change &lt;= -5%</t>
+  </si>
+  <si>
+    <t>Lnd. Rate    S. F.</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Lnd. S. F.</t>
+  </si>
+  <si>
+    <t>Year Built</t>
+  </si>
+  <si>
+    <t>Nbhd.</t>
+  </si>
+  <si>
+    <t>Run ID (condo):</t>
+  </si>
+  <si>
+    <t>Total        Bld. S. F.</t>
+  </si>
+  <si>
+    <t>Condo Non-Livable Space</t>
+  </si>
+  <si>
+    <t>Condo Unit S. F.</t>
+  </si>
+  <si>
+    <t>Condo Bld. # Sales (Past 5 Years)</t>
+  </si>
+  <si>
+    <t>Condo Building ID (PIN10)</t>
+  </si>
+  <si>
+    <t>Tieback Percent Ownership</t>
+  </si>
+  <si>
+    <t>Condo Potential Common Area</t>
+  </si>
+  <si>
+    <t>% Ownership Sum Not Equal to 1</t>
+  </si>
+  <si>
+    <t>Unit Rate   S. F.</t>
+  </si>
+  <si>
+    <t>Unit Rate    S. F.</t>
+  </si>
+  <si>
+    <t>PIN10</t>
+  </si>
+  <si>
+    <t>Total Res. % Ownership</t>
+  </si>
+  <si>
+    <t>Num. Livable PINs</t>
+  </si>
+  <si>
+    <t>Num. Non-Livable PINs</t>
+  </si>
+  <si>
+    <t>Building Total FMV</t>
+  </si>
+  <si>
+    <t>Bld. Total S. F.</t>
+  </si>
+  <si>
+    <t>Aggregated stats by building (PIN10)</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 1</t>
+  </si>
+  <si>
+    <t>Non-Arm's-Length Sale Flag 2</t>
+  </si>
+  <si>
+    <t>Characteristics</t>
+  </si>
+  <si>
+    <t>PIN Information</t>
+  </si>
+  <si>
+    <t>Change In Value</t>
+  </si>
+  <si>
+    <t>Sales Information</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Valuations Notes</t>
+  </si>
+  <si>
+    <t>Lnd. &gt;= 95% in Town</t>
+  </si>
+  <si>
     <t>Value Unchanged</t>
   </si>
   <si>
-    <t>YoY Change &gt;= 50%</t>
-  </si>
-  <si>
-    <t>YoY Change &lt;= -5%</t>
-  </si>
-  <si>
-    <t>Lnd. Rate    S. F.</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>Lnd. S. F.</t>
-  </si>
-  <si>
-    <t>Year Built</t>
-  </si>
-  <si>
-    <t>Nbhd.</t>
-  </si>
-  <si>
-    <t>Run ID (condo):</t>
-  </si>
-  <si>
-    <t>Total        Bld. S. F.</t>
-  </si>
-  <si>
-    <t>Condo Non-Livable Space</t>
-  </si>
-  <si>
-    <t>Condo Unit S. F.</t>
-  </si>
-  <si>
-    <t>Condo Bld. # Sales (Past 5 Years)</t>
-  </si>
-  <si>
-    <t>Condo Building ID (PIN10)</t>
-  </si>
-  <si>
-    <t>Tieback Percent Ownership</t>
-  </si>
-  <si>
-    <t>Condo Potential Common Area</t>
-  </si>
-  <si>
-    <t>% Ownership Sum Not Equal to 1</t>
-  </si>
-  <si>
-    <t>Unit Rate   S. F.</t>
-  </si>
-  <si>
-    <t>Unit Rate    S. F.</t>
-  </si>
-  <si>
-    <t>PIN10</t>
-  </si>
-  <si>
-    <t>Total Res. % Ownership</t>
-  </si>
-  <si>
-    <t>Num. Livable PINs</t>
-  </si>
-  <si>
-    <t>Num. Non-Livable PINs</t>
-  </si>
-  <si>
-    <t>Building Total FMV</t>
-  </si>
-  <si>
-    <t>Bld. Total S. F.</t>
-  </si>
-  <si>
-    <t>Aggregated stats by building (PIN10)</t>
+    <t>Summary statistics broken out by neighborhood</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Class</t>
+  </si>
+  <si>
+    <t>Total AV</t>
+  </si>
+  <si>
+    <t>AV Difference</t>
+  </si>
+  <si>
+    <t>Min of Total AV</t>
+  </si>
+  <si>
+    <t>Average of Total AV</t>
+  </si>
+  <si>
+    <t>Max of Total AV</t>
+  </si>
+  <si>
+    <t>Average of AV Difference</t>
+  </si>
+  <si>
+    <t>Average of YoY ∆ %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,8 +495,16 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +523,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -377,6 +650,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -384,7 +672,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -396,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -406,44 +694,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -453,6 +783,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,6 +806,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9CCFC"/>
+      <color rgb="FFFFD1D1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -473,6 +821,355 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.444692708334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="pin_detail_range"/>
+  </cacheSource>
+  <cacheFields count="50">
+    <cacheField name="PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Class" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nbhd." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Street Address" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Municipality" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Building ID (PIN10)" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback Key PIN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Tieback Percent Ownership" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Unit Rate   S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Total" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Before Rounding" numFmtId="44">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate Original" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. Rate     Effective" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Unit Rate    S. F." numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. % of Tot." numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ $" numFmtId="164">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY ∆ %" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Valuations Notes" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 1" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Date 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Amount 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Non-Arm's-Length Sale Flag 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Doc. 2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Year Built" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total        Bld. S. F." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stories" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. S. F." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Unit S. F." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Non-Livable Space" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Bld. # Sales (Past 5 Years)" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Condo Potential Common Area" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="% Ownership Sum Not Equal to 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Multi-Land" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Lnd. &gt;= 95% in Town" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Land Value Capped" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Value Unchanged" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &gt;= 50%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Total AV" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="AV Difference" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="50">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="3"/>
+    <dataField name="Min of Total AV" fld="48" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of Total AV" fld="48" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max of Total AV" fld="48" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of AV Difference" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average of YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -771,14 +1468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA1048575"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -786,15 +1483,16 @@
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="6" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="15.375" customWidth="1"/>
     <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
     <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
     <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
     <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
     <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
     <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
@@ -802,31 +1500,37 @@
     <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="24" width="11" style="11"/>
-    <col min="25" max="25" width="10.375" customWidth="1"/>
-    <col min="26" max="26" width="13" style="10" customWidth="1"/>
-    <col min="27" max="28" width="13" style="18" customWidth="1"/>
-    <col min="29" max="29" width="13" style="10" customWidth="1"/>
-    <col min="30" max="30" width="13" style="18" customWidth="1"/>
-    <col min="34" max="34" width="11" style="13"/>
-    <col min="36" max="36" width="15.625" customWidth="1"/>
-    <col min="37" max="37" width="17.375" customWidth="1"/>
-    <col min="38" max="39" width="15.625" customWidth="1"/>
-    <col min="40" max="40" width="12.625" customWidth="1"/>
-    <col min="42" max="42" width="14" customWidth="1"/>
-    <col min="43" max="43" width="11.875" customWidth="1"/>
-    <col min="44" max="44" width="10.875" customWidth="1"/>
+    <col min="25" max="25" width="21.125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="13" customWidth="1"/>
+    <col min="27" max="27" width="13" style="10" customWidth="1"/>
+    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="30" width="13" style="16" customWidth="1"/>
+    <col min="31" max="31" width="13" style="10" customWidth="1"/>
+    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
+    <col min="33" max="33" width="13" style="16" customWidth="1"/>
+    <col min="37" max="37" width="11" style="13"/>
+    <col min="39" max="39" width="15.625" customWidth="1"/>
+    <col min="40" max="40" width="17.375" customWidth="1"/>
+    <col min="41" max="42" width="15.625" customWidth="1"/>
+    <col min="43" max="43" width="12.625" customWidth="1"/>
+    <col min="44" max="44" width="13.25" customWidth="1"/>
+    <col min="45" max="45" width="14.125" customWidth="1"/>
+    <col min="47" max="47" width="14" customWidth="1"/>
+    <col min="48" max="48" width="14.875" customWidth="1"/>
+    <col min="49" max="49" width="11.875" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -871,8 +1575,14 @@
       <c r="AY1" s="5"/>
       <c r="AZ1" s="5"/>
       <c r="BA1" s="5"/>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -897,20 +1607,23 @@
       <c r="V2"/>
       <c r="W2"/>
       <c r="X2"/>
-      <c r="Z2"/>
+      <c r="Y2"/>
       <c r="AA2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
-      <c r="AH2"/>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AK2"/>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -930,14 +1643,17 @@
       <c r="V3"/>
       <c r="W3"/>
       <c r="X3"/>
-      <c r="Z3"/>
+      <c r="Y3"/>
       <c r="AA3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
-      <c r="AH3"/>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AK3"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -956,49 +1672,80 @@
       <c r="V4"/>
       <c r="W4"/>
       <c r="X4"/>
-      <c r="Z4"/>
+      <c r="Y4"/>
       <c r="AA4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
-      <c r="AH4"/>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="H5"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="29"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AH5"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="26"/>
-      <c r="AQ5" s="26"/>
-      <c r="AR5" s="26"/>
-    </row>
-    <row r="6" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AK4"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B5" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN5" s="30"/>
+      <c r="AO5" s="30"/>
+      <c r="AP5" s="30"/>
+      <c r="AQ5" s="30"/>
+      <c r="AR5" s="30"/>
+      <c r="AS5" s="30"/>
+      <c r="AT5" s="30"/>
+      <c r="AU5" s="30"/>
+      <c r="AV5" s="31"/>
+      <c r="AW5" s="19"/>
+      <c r="AX5" s="19"/>
+    </row>
+    <row r="6" spans="1:59" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>9</v>
@@ -1015,28 +1762,28 @@
         <v>10</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>37</v>
+      <c r="H6" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>8</v>
@@ -1044,11 +1791,11 @@
       <c r="O6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>5</v>
@@ -1060,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>6</v>
@@ -1071,268 +1818,291 @@
       <c r="X6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Y6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="AA6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AD6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="AE6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AE6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI6" s="9" t="s">
+      <c r="AN6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AJ6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AM6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN6" s="8" t="s">
+      <c r="AQ6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AV6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AR6" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="1048519" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="32:32" x14ac:dyDescent="0.25">
-      <c r="AF1048575" s="13"/>
+      <c r="AW6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
+      <c r="AI1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="AH5:AL5"/>
+    <mergeCell ref="AM5:AV5"/>
+    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="B5:H5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
-    <mergeCell ref="AI5:AR5"/>
     <mergeCell ref="O5:V5"/>
+    <mergeCell ref="W5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1048573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="5" max="6" width="11.625" customWidth="1"/>
     <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
@@ -1343,14 +2113,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -1364,17 +2134,31 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3"/>
-      <c r="K3"/>
+      <c r="B3" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="48"/>
+      <c r="L3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
@@ -1383,19 +2167,19 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -1404,10 +2188,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
@@ -1580,13 +2364,109 @@
     </row>
     <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048573" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4264-9F60-48E3-A5EA-D04C0BA089E2}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalize desk review workbooks
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2366FE96-8444-474B-9653-F87BFABDD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486E6F9-2481-491A-98E0-DB4487C1059C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AX$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AZ$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,6 +47,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jean Cochrane</author>
+    <author>Daniel F. Snow</author>
   </authors>
   <commentList>
     <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
@@ -63,7 +64,113 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AD6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Condo buildings often includes sales of multiple parcels, usually a unit and deeded parking space. This field captures the number of parcels for a given sale.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WARNING:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Multi-PIN sales have their prices adjusted such that the sale price reflects the value of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>only the unit</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, not the unit + parking.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Condo buildings often includes sales of multiple parcels, usually a unit and deeded parking space. This field captures the number of parcels for a given sale.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WARNING:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Multi-PIN sales have their prices adjusted such that the sale price reflects the value of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>only the unit</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, not the unit + parking.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
           <rPr>
@@ -76,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
@@ -90,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
       <text>
         <r>
           <rPr>
@@ -103,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -117,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -131,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -144,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -157,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -170,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -183,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -225,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>PIN</t>
   </si>
@@ -416,9 +523,6 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Count of Class</t>
-  </si>
-  <si>
     <t>Total AV</t>
   </si>
   <si>
@@ -438,6 +542,12 @@
   </si>
   <si>
     <t>Average of YoY ∆ %</t>
+  </si>
+  <si>
+    <t>Sale Num. Parcels 1</t>
+  </si>
+  <si>
+    <t>Sale Num. Parcels 2</t>
   </si>
 </sst>
 </file>
@@ -451,7 +561,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -463,13 +573,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,6 +605,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -668,11 +785,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -684,7 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,10 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -720,11 +834,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,13 +847,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -761,7 +874,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -776,13 +889,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,7 +937,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.444692708334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.485052083335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -833,9 +946,7 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Class" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
-        <m/>
-      </sharedItems>
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Nbhd." numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
@@ -996,7 +1107,7 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
     <m/>
-    <x v="0"/>
+    <m/>
     <x v="0"/>
     <m/>
     <m/>
@@ -1050,16 +1161,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="50">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -1114,15 +1220,11 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="1">
     <field x="2"/>
-    <field x="1"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="2">
     <i>
-      <x/>
-    </i>
-    <i r="1">
       <x/>
     </i>
     <i t="grand">
@@ -1132,7 +1234,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="5">
     <i>
       <x/>
     </i>
@@ -1148,12 +1250,8 @@
     <i i="4">
       <x v="4"/>
     </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
   </colItems>
-  <dataFields count="6">
-    <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="3"/>
+  <dataFields count="5">
     <dataField name="Min of Total AV" fld="48" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average of Total AV" fld="48" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Max of Total AV" fld="48" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
@@ -1469,13 +1567,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG1048575"/>
+  <dimension ref="A1:BI1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1504,33 +1602,33 @@
     <col min="26" max="26" width="13" customWidth="1"/>
     <col min="27" max="27" width="13" style="10" customWidth="1"/>
     <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
-    <col min="29" max="30" width="13" style="16" customWidth="1"/>
-    <col min="31" max="31" width="13" style="10" customWidth="1"/>
-    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
-    <col min="33" max="33" width="13" style="16" customWidth="1"/>
-    <col min="37" max="37" width="11" style="13"/>
-    <col min="39" max="39" width="15.625" customWidth="1"/>
-    <col min="40" max="40" width="17.375" customWidth="1"/>
-    <col min="41" max="42" width="15.625" customWidth="1"/>
-    <col min="43" max="43" width="12.625" customWidth="1"/>
-    <col min="44" max="44" width="13.25" customWidth="1"/>
-    <col min="45" max="45" width="14.125" customWidth="1"/>
-    <col min="47" max="47" width="14" customWidth="1"/>
-    <col min="48" max="48" width="14.875" customWidth="1"/>
-    <col min="49" max="49" width="11.875" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="10.875" hidden="1" customWidth="1"/>
+    <col min="29" max="31" width="13" style="16" customWidth="1"/>
+    <col min="32" max="32" width="13" style="10" customWidth="1"/>
+    <col min="33" max="34" width="18.625" style="10" customWidth="1"/>
+    <col min="35" max="35" width="13" style="16" customWidth="1"/>
+    <col min="39" max="39" width="11" style="13"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="17.375" customWidth="1"/>
+    <col min="43" max="44" width="15.625" customWidth="1"/>
+    <col min="45" max="45" width="12.625" customWidth="1"/>
+    <col min="46" max="46" width="13.25" customWidth="1"/>
+    <col min="47" max="47" width="14.125" customWidth="1"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
+    <col min="50" max="50" width="14.875" customWidth="1"/>
+    <col min="51" max="51" width="11.875" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1581,8 +1679,10 @@
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1615,15 +1715,17 @@
       <c r="AE2"/>
       <c r="AF2"/>
       <c r="AG2"/>
-      <c r="AK2"/>
-    </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AM2"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1651,9 +1753,11 @@
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AG3"/>
-      <c r="AK3"/>
-    </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AM3"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1680,72 +1784,76 @@
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AK4"/>
-    </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AM4"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="20" t="s">
+      <c r="X5" s="45"/>
+      <c r="Y5" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" s="32" t="s">
+      <c r="Z5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="33"/>
-      <c r="AE5" s="33"/>
-      <c r="AF5" s="33"/>
-      <c r="AG5" s="35"/>
-      <c r="AH5" s="26" t="s">
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="32"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="31"/>
+      <c r="AG5" s="31"/>
+      <c r="AH5" s="32"/>
+      <c r="AI5" s="33"/>
+      <c r="AJ5" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="28"/>
-      <c r="AM5" s="29" t="s">
+      <c r="AK5" s="25"/>
+      <c r="AL5" s="25"/>
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AN5" s="30"/>
-      <c r="AO5" s="30"/>
-      <c r="AP5" s="30"/>
-      <c r="AQ5" s="30"/>
-      <c r="AR5" s="30"/>
-      <c r="AS5" s="30"/>
-      <c r="AT5" s="30"/>
-      <c r="AU5" s="30"/>
-      <c r="AV5" s="31"/>
-      <c r="AW5" s="19"/>
-      <c r="AX5" s="19"/>
-    </row>
-    <row r="6" spans="1:59" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="29"/>
+      <c r="AY5" s="18"/>
+      <c r="AZ5" s="18"/>
+    </row>
+    <row r="6" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1830,249 +1938,255 @@
       <c r="AB6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AC6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AG6" s="4" t="s">
+      <c r="AH6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AI6" s="3" t="s">
+      <c r="AK6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AL6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AM6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AN6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AM6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AP6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AQ6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AS6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AV6" s="14" t="s">
+      <c r="AX6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AW6" s="2" t="s">
+      <c r="AY6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AX6" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048575" s="13"/>
+    </row>
+    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AH5:AL5"/>
-    <mergeCell ref="AM5:AV5"/>
-    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="AJ5:AN5"/>
+    <mergeCell ref="AO5:AX5"/>
+    <mergeCell ref="Z5:AI5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
@@ -2094,7 +2208,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2113,14 +2227,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -2134,24 +2248,24 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="28"/>
+      <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2380,39 +2494,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4264-9F60-48E3-A5EA-D04C0BA089E2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4:F4"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" max="3" activeRow="3" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" fieldPosition="0">
+          <references count="1">
+            <reference field="2" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
@@ -2426,42 +2548,26 @@
       <c r="F3" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="25"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="24"/>
+      <c r="A5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="25"/>
+      <c r="F5" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Finalize desk review workbook tweaks
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486E6F9-2481-491A-98E0-DB4487C1059C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F1241-156A-4263-93F8-102CD557789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AZ$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AY$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
           <rPr>
@@ -183,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
@@ -197,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -224,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -238,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -251,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -264,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -277,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -290,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>PIN</t>
   </si>
@@ -355,9 +355,6 @@
     <t>Lnd. % of Tot.</t>
   </si>
   <si>
-    <t>Stories</t>
-  </si>
-  <si>
     <t>Lnd. % of Total</t>
   </si>
   <si>
@@ -529,25 +526,25 @@
     <t>AV Difference</t>
   </si>
   <si>
-    <t>Min of Total AV</t>
-  </si>
-  <si>
-    <t>Average of Total AV</t>
-  </si>
-  <si>
-    <t>Max of Total AV</t>
-  </si>
-  <si>
-    <t>Average of AV Difference</t>
-  </si>
-  <si>
-    <t>Average of YoY ∆ %</t>
-  </si>
-  <si>
     <t>Sale Num. Parcels 1</t>
   </si>
   <si>
     <t>Sale Num. Parcels 2</t>
+  </si>
+  <si>
+    <t>Average AV Difference</t>
+  </si>
+  <si>
+    <t>Average YoY ∆ %</t>
+  </si>
+  <si>
+    <t>Max AV</t>
+  </si>
+  <si>
+    <t>Average AV</t>
+  </si>
+  <si>
+    <t>Min AV</t>
   </si>
 </sst>
 </file>
@@ -937,11 +934,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.485052083335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.642089004628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="50">
+  <cacheFields count="51">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1031,6 +1028,9 @@
     <cacheField name="Sale Doc. 1" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
+    <cacheField name="Sale Num. Parcels 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
     <cacheField name="Sale Date 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1040,16 +1040,16 @@
     <cacheField name="Non-Arm's-Length Sale Flag 2" numFmtId="42">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Sale Doc. 2" numFmtId="0">
+    <cacheField name="Sale Doc. 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Num. Parcels 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Year Built" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total        Bld. S. F." numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Stories" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Lnd. S. F." numFmtId="37">
@@ -1156,14 +1156,15 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="50">
+  <pivotFields count="51">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -1193,6 +1194,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1252,11 +1254,11 @@
     </i>
   </colItems>
   <dataFields count="5">
-    <dataField name="Min of Total AV" fld="48" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="48" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="48" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+    <dataField name="Min AV" fld="49" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max AV" fld="49" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV Difference" fld="50" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1567,7 +1569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI1048575"/>
+  <dimension ref="A1:BH1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -1606,20 +1608,20 @@
     <col min="32" max="32" width="13" style="10" customWidth="1"/>
     <col min="33" max="34" width="18.625" style="10" customWidth="1"/>
     <col min="35" max="35" width="13" style="16" customWidth="1"/>
-    <col min="39" max="39" width="11" style="13"/>
-    <col min="41" max="41" width="15.625" customWidth="1"/>
-    <col min="42" max="42" width="17.375" customWidth="1"/>
-    <col min="43" max="44" width="15.625" customWidth="1"/>
-    <col min="45" max="45" width="12.625" customWidth="1"/>
-    <col min="46" max="46" width="13.25" customWidth="1"/>
-    <col min="47" max="47" width="14.125" customWidth="1"/>
-    <col min="49" max="49" width="14" customWidth="1"/>
-    <col min="50" max="50" width="14.875" customWidth="1"/>
-    <col min="51" max="51" width="11.875" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="10.875" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="11" style="13"/>
+    <col min="40" max="40" width="15.625" customWidth="1"/>
+    <col min="41" max="41" width="17.375" customWidth="1"/>
+    <col min="42" max="43" width="15.625" customWidth="1"/>
+    <col min="44" max="44" width="12.625" customWidth="1"/>
+    <col min="45" max="45" width="13.25" customWidth="1"/>
+    <col min="46" max="46" width="14.125" customWidth="1"/>
+    <col min="48" max="48" width="14" customWidth="1"/>
+    <col min="49" max="49" width="14.875" customWidth="1"/>
+    <col min="50" max="50" width="11.875" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1680,9 +1682,8 @@
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
       <c r="BH1" s="5"/>
-      <c r="BI1" s="5"/>
-    </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1717,11 +1718,11 @@
       <c r="AG2"/>
       <c r="AH2"/>
       <c r="AI2"/>
-      <c r="AM2"/>
-    </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AL2"/>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
@@ -1755,9 +1756,9 @@
       <c r="AG3"/>
       <c r="AH3"/>
       <c r="AI3"/>
-      <c r="AM3"/>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AL3"/>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1786,11 +1787,11 @@
       <c r="AG4"/>
       <c r="AH4"/>
       <c r="AI4"/>
-      <c r="AM4"/>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="AL4"/>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -1813,14 +1814,14 @@
       <c r="U5" s="42"/>
       <c r="V5" s="43"/>
       <c r="W5" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X5" s="45"/>
       <c r="Y5" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Z5" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA5" s="31"/>
       <c r="AB5" s="31"/>
@@ -1832,15 +1833,15 @@
       <c r="AH5" s="32"/>
       <c r="AI5" s="33"/>
       <c r="AJ5" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AK5" s="25"/>
       <c r="AL5" s="25"/>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="27" t="s">
-        <v>54</v>
-      </c>
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO5" s="28"/>
       <c r="AP5" s="28"/>
       <c r="AQ5" s="28"/>
       <c r="AR5" s="28"/>
@@ -1848,12 +1849,11 @@
       <c r="AT5" s="28"/>
       <c r="AU5" s="28"/>
       <c r="AV5" s="28"/>
-      <c r="AW5" s="28"/>
-      <c r="AX5" s="29"/>
+      <c r="AW5" s="29"/>
+      <c r="AX5" s="18"/>
       <c r="AY5" s="18"/>
-      <c r="AZ5" s="18"/>
-    </row>
-    <row r="6" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:60" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1861,61 +1861,61 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="S6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="U6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>6</v>
@@ -1927,88 +1927,85 @@
         <v>3</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Z6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AD6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AC6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD6" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="AI6" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AK6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AL6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AN6" s="14" t="s">
+      <c r="AO6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AO6" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="AP6" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AQ6" s="9" t="s">
         <v>37</v>
       </c>
       <c r="AR6" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AS6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AV6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AW6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AX6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AY6" s="2" t="s">
+      <c r="AX6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY6" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
@@ -2184,8 +2181,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AJ5:AN5"/>
-    <mergeCell ref="AO5:AX5"/>
+    <mergeCell ref="AJ5:AM5"/>
+    <mergeCell ref="AN5:AW5"/>
     <mergeCell ref="Z5:AI5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B1:I1"/>
@@ -2228,7 +2225,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -2259,41 +2256,41 @@
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
       <c r="J3" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="46"/>
       <c r="L3" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -2302,10 +2299,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
@@ -2497,31 +2494,19 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" max="3" activeRow="3" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" fieldPosition="0">
-          <references count="1">
-            <reference field="2" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2531,27 +2516,27 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -2561,7 +2546,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>

</xml_diff>

<commit_message>
Finalize desk review workbooks (#34)
* Finalize desk review workbooks

* Add num_parcels to export

* Finalize desk review workbook tweaks

---------

Co-authored-by: William Ridgeway <10358980+wrridgeway@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2366FE96-8444-474B-9653-F87BFABDD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F1241-156A-4263-93F8-102CD557789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AX$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AY$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,6 +47,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jean Cochrane</author>
+    <author>Daniel F. Snow</author>
   </authors>
   <commentList>
     <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
@@ -63,7 +64,113 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AD6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Condo buildings often includes sales of multiple parcels, usually a unit and deeded parking space. This field captures the number of parcels for a given sale.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WARNING:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Multi-PIN sales have their prices adjusted such that the sale price reflects the value of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>only the unit</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, not the unit + parking.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Condo buildings often includes sales of multiple parcels, usually a unit and deeded parking space. This field captures the number of parcels for a given sale.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WARNING:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Multi-PIN sales have their prices adjusted such that the sale price reflects the value of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>only the unit</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, not the unit + parking.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
           <rPr>
@@ -76,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
@@ -90,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
       <text>
         <r>
           <rPr>
@@ -103,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -117,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -131,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -144,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -157,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -170,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -183,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -225,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>PIN</t>
   </si>
@@ -248,9 +355,6 @@
     <t>Lnd. % of Tot.</t>
   </si>
   <si>
-    <t>Stories</t>
-  </si>
-  <si>
     <t>Lnd. % of Total</t>
   </si>
   <si>
@@ -416,28 +520,31 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Count of Class</t>
-  </si>
-  <si>
     <t>Total AV</t>
   </si>
   <si>
     <t>AV Difference</t>
   </si>
   <si>
-    <t>Min of Total AV</t>
-  </si>
-  <si>
-    <t>Average of Total AV</t>
-  </si>
-  <si>
-    <t>Max of Total AV</t>
-  </si>
-  <si>
-    <t>Average of AV Difference</t>
-  </si>
-  <si>
-    <t>Average of YoY ∆ %</t>
+    <t>Sale Num. Parcels 1</t>
+  </si>
+  <si>
+    <t>Sale Num. Parcels 2</t>
+  </si>
+  <si>
+    <t>Average AV Difference</t>
+  </si>
+  <si>
+    <t>Average YoY ∆ %</t>
+  </si>
+  <si>
+    <t>Max AV</t>
+  </si>
+  <si>
+    <t>Average AV</t>
+  </si>
+  <si>
+    <t>Min AV</t>
   </si>
 </sst>
 </file>
@@ -451,7 +558,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -463,13 +570,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,6 +602,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -668,11 +782,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -684,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,10 +823,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -720,11 +831,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,13 +844,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -761,7 +871,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -776,13 +886,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,18 +934,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45335.444692708334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.642089004628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="50">
+  <cacheFields count="51">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Class" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
-        <m/>
-      </sharedItems>
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Nbhd." numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
@@ -920,6 +1028,9 @@
     <cacheField name="Sale Doc. 1" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
+    <cacheField name="Sale Num. Parcels 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
     <cacheField name="Sale Date 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -929,16 +1040,16 @@
     <cacheField name="Non-Arm's-Length Sale Flag 2" numFmtId="42">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Sale Doc. 2" numFmtId="0">
+    <cacheField name="Sale Doc. 2" numFmtId="42">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale Num. Parcels 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Year Built" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total        Bld. S. F." numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Stories" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Lnd. S. F." numFmtId="37">
@@ -996,8 +1107,9 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
     <m/>
+    <m/>
     <x v="0"/>
-    <x v="0"/>
+    <m/>
     <m/>
     <m/>
     <m/>
@@ -1050,16 +1162,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="50">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="51">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -1111,18 +1218,15 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="1">
     <field x="2"/>
-    <field x="1"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="2">
     <i>
-      <x/>
-    </i>
-    <i r="1">
       <x/>
     </i>
     <i t="grand">
@@ -1132,7 +1236,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="5">
     <i>
       <x/>
     </i>
@@ -1148,17 +1252,13 @@
     <i i="4">
       <x v="4"/>
     </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
   </colItems>
-  <dataFields count="6">
-    <dataField name="Count of Class" fld="1" subtotal="count" baseField="2" baseItem="0" numFmtId="3"/>
-    <dataField name="Min of Total AV" fld="48" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of Total AV" fld="48" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max of Total AV" fld="48" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of AV Difference" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average of YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
+  <dataFields count="5">
+    <dataField name="Min AV" fld="49" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max AV" fld="49" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV Difference" fld="50" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1469,13 +1569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG1048575"/>
+  <dimension ref="A1:BH1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1504,33 +1604,33 @@
     <col min="26" max="26" width="13" customWidth="1"/>
     <col min="27" max="27" width="13" style="10" customWidth="1"/>
     <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
-    <col min="29" max="30" width="13" style="16" customWidth="1"/>
-    <col min="31" max="31" width="13" style="10" customWidth="1"/>
-    <col min="32" max="32" width="18.625" style="10" customWidth="1"/>
-    <col min="33" max="33" width="13" style="16" customWidth="1"/>
-    <col min="37" max="37" width="11" style="13"/>
-    <col min="39" max="39" width="15.625" customWidth="1"/>
-    <col min="40" max="40" width="17.375" customWidth="1"/>
-    <col min="41" max="42" width="15.625" customWidth="1"/>
-    <col min="43" max="43" width="12.625" customWidth="1"/>
-    <col min="44" max="44" width="13.25" customWidth="1"/>
-    <col min="45" max="45" width="14.125" customWidth="1"/>
-    <col min="47" max="47" width="14" customWidth="1"/>
-    <col min="48" max="48" width="14.875" customWidth="1"/>
-    <col min="49" max="49" width="11.875" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="10.875" hidden="1" customWidth="1"/>
+    <col min="29" max="31" width="13" style="16" customWidth="1"/>
+    <col min="32" max="32" width="13" style="10" customWidth="1"/>
+    <col min="33" max="34" width="18.625" style="10" customWidth="1"/>
+    <col min="35" max="35" width="13" style="16" customWidth="1"/>
+    <col min="38" max="38" width="11" style="13"/>
+    <col min="40" max="40" width="15.625" customWidth="1"/>
+    <col min="41" max="41" width="17.375" customWidth="1"/>
+    <col min="42" max="43" width="15.625" customWidth="1"/>
+    <col min="44" max="44" width="12.625" customWidth="1"/>
+    <col min="45" max="45" width="13.25" customWidth="1"/>
+    <col min="46" max="46" width="14.125" customWidth="1"/>
+    <col min="48" max="48" width="14" customWidth="1"/>
+    <col min="49" max="49" width="14.875" customWidth="1"/>
+    <col min="50" max="50" width="11.875" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1581,8 +1681,9 @@
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH1" s="5"/>
+    </row>
+    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1615,15 +1716,17 @@
       <c r="AE2"/>
       <c r="AF2"/>
       <c r="AG2"/>
-      <c r="AK2"/>
-    </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AL2"/>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+        <v>29</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1651,9 +1754,11 @@
       <c r="AE3"/>
       <c r="AF3"/>
       <c r="AG3"/>
-      <c r="AK3"/>
-    </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AL3"/>
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1680,72 +1785,75 @@
       <c r="AE4"/>
       <c r="AF4"/>
       <c r="AG4"/>
-      <c r="AK4"/>
-    </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AL4"/>
+    </row>
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46" t="s">
+      <c r="X5" s="45"/>
+      <c r="Y5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z5" s="32" t="s">
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="32"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="31"/>
+      <c r="AG5" s="31"/>
+      <c r="AH5" s="32"/>
+      <c r="AI5" s="33"/>
+      <c r="AJ5" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK5" s="25"/>
+      <c r="AL5" s="25"/>
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="33"/>
-      <c r="AE5" s="33"/>
-      <c r="AF5" s="33"/>
-      <c r="AG5" s="35"/>
-      <c r="AH5" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="28"/>
-      <c r="AM5" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN5" s="30"/>
-      <c r="AO5" s="30"/>
-      <c r="AP5" s="30"/>
-      <c r="AQ5" s="30"/>
-      <c r="AR5" s="30"/>
-      <c r="AS5" s="30"/>
-      <c r="AT5" s="30"/>
-      <c r="AU5" s="30"/>
-      <c r="AV5" s="31"/>
-      <c r="AW5" s="19"/>
-      <c r="AX5" s="19"/>
-    </row>
-    <row r="6" spans="1:59" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="29"/>
+      <c r="AX5" s="18"/>
+      <c r="AY5" s="18"/>
+    </row>
+    <row r="6" spans="1:60" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1753,61 +1861,61 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="S6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="U6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>6</v>
@@ -1819,260 +1927,263 @@
         <v>3</v>
       </c>
       <c r="Y6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="Z6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AT6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AW6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AV6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AW6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AX6" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="1048519" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="35:35" x14ac:dyDescent="0.25">
-      <c r="AI1048575" s="13"/>
+      <c r="AX6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
+      <c r="AK1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AH5:AL5"/>
-    <mergeCell ref="AM5:AV5"/>
-    <mergeCell ref="Z5:AG5"/>
+    <mergeCell ref="AJ5:AM5"/>
+    <mergeCell ref="AN5:AW5"/>
+    <mergeCell ref="Z5:AI5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
@@ -2094,7 +2205,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2113,14 +2224,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -2134,52 +2245,52 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="28"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -2188,10 +2299,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
@@ -2380,88 +2491,68 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4264-9F60-48E3-A5EA-D04C0BA089E2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.625" customWidth="1"/>
     <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="25"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="25"/>
+      <c r="F5" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add Sale Ratio column to desk review workbooks
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F1241-156A-4263-93F8-102CD557789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C62BF-04D4-416B-988C-0602B5F8683A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AY$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AZ$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -50,7 +50,20 @@
     <author>Daniel F. Snow</author>
   </authors>
   <commentList>
-    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{2D923700-2902-4CB6-8749-A7F11C03AEC1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If a recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
       <text>
         <r>
           <rPr>
@@ -64,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
+    <comment ref="AE6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
       <text>
         <r>
           <rPr>
@@ -117,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
+    <comment ref="AJ6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
       <text>
         <r>
           <rPr>
@@ -170,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
           <rPr>
@@ -183,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
@@ -197,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
       <text>
         <r>
           <rPr>
@@ -210,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -224,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -238,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -251,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -264,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -277,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -290,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -332,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>PIN</t>
   </si>
@@ -545,6 +558,9 @@
   </si>
   <si>
     <t>Min AV</t>
+  </si>
+  <si>
+    <t>Sale Ratio</t>
   </si>
 </sst>
 </file>
@@ -786,7 +802,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -906,6 +922,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -934,7 +956,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.642089004628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45351.582175115742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1569,13 +1591,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH1048575"/>
+  <dimension ref="A1:BI1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1598,30 +1620,30 @@
     <col min="19" max="19" width="11" style="10"/>
     <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
     <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
-    <col min="23" max="23" width="11" style="12"/>
-    <col min="24" max="24" width="11" style="11"/>
-    <col min="25" max="25" width="21.125" style="11" customWidth="1"/>
-    <col min="26" max="26" width="13" customWidth="1"/>
-    <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
-    <col min="29" max="31" width="13" style="16" customWidth="1"/>
-    <col min="32" max="32" width="13" style="10" customWidth="1"/>
-    <col min="33" max="34" width="18.625" style="10" customWidth="1"/>
-    <col min="35" max="35" width="13" style="16" customWidth="1"/>
-    <col min="38" max="38" width="11" style="13"/>
-    <col min="40" max="40" width="15.625" customWidth="1"/>
-    <col min="41" max="41" width="17.375" customWidth="1"/>
-    <col min="42" max="43" width="15.625" customWidth="1"/>
-    <col min="44" max="44" width="12.625" customWidth="1"/>
-    <col min="45" max="45" width="13.25" customWidth="1"/>
-    <col min="46" max="46" width="14.125" customWidth="1"/>
-    <col min="48" max="48" width="14" customWidth="1"/>
-    <col min="49" max="49" width="14.875" customWidth="1"/>
-    <col min="50" max="50" width="11.875" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="10.875" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="11" style="12"/>
+    <col min="25" max="25" width="11" style="11"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13" customWidth="1"/>
+    <col min="28" max="28" width="13" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="30" max="32" width="13" style="16" customWidth="1"/>
+    <col min="33" max="33" width="13" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
+    <col min="36" max="36" width="13" style="16" customWidth="1"/>
+    <col min="39" max="39" width="11" style="13"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="17.375" customWidth="1"/>
+    <col min="43" max="44" width="15.625" customWidth="1"/>
+    <col min="45" max="45" width="12.625" customWidth="1"/>
+    <col min="46" max="46" width="13.25" customWidth="1"/>
+    <col min="47" max="47" width="14.125" customWidth="1"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
+    <col min="50" max="50" width="14.875" customWidth="1"/>
+    <col min="51" max="51" width="11.875" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1682,8 +1704,9 @@
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
       <c r="BH1" s="5"/>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BI1" s="5"/>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1709,7 +1732,7 @@
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="AA2"/>
+      <c r="Z2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
@@ -1718,9 +1741,10 @@
       <c r="AG2"/>
       <c r="AH2"/>
       <c r="AI2"/>
-      <c r="AL2"/>
-    </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AJ2"/>
+      <c r="AM2"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1747,7 +1771,7 @@
       <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
-      <c r="AA3"/>
+      <c r="Z3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
@@ -1756,9 +1780,10 @@
       <c r="AG3"/>
       <c r="AH3"/>
       <c r="AI3"/>
-      <c r="AL3"/>
-    </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AJ3"/>
+      <c r="AM3"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1778,7 +1803,7 @@
       <c r="W4"/>
       <c r="X4"/>
       <c r="Y4"/>
-      <c r="AA4"/>
+      <c r="Z4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
@@ -1787,9 +1812,10 @@
       <c r="AG4"/>
       <c r="AH4"/>
       <c r="AI4"/>
-      <c r="AL4"/>
-    </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AJ4"/>
+      <c r="AM4"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>50</v>
       </c>
@@ -1816,32 +1842,32 @@
       <c r="W5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="19" t="s">
+      <c r="X5" s="48"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="Z5" s="30" t="s">
+      <c r="AA5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="AA5" s="31"/>
       <c r="AB5" s="31"/>
-      <c r="AC5" s="32"/>
+      <c r="AC5" s="31"/>
       <c r="AD5" s="32"/>
-      <c r="AE5" s="31"/>
+      <c r="AE5" s="32"/>
       <c r="AF5" s="31"/>
       <c r="AG5" s="31"/>
-      <c r="AH5" s="32"/>
-      <c r="AI5" s="33"/>
-      <c r="AJ5" s="24" t="s">
+      <c r="AH5" s="31"/>
+      <c r="AI5" s="32"/>
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AK5" s="25"/>
       <c r="AL5" s="25"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="27" t="s">
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" s="28"/>
       <c r="AP5" s="28"/>
       <c r="AQ5" s="28"/>
       <c r="AR5" s="28"/>
@@ -1849,11 +1875,12 @@
       <c r="AT5" s="28"/>
       <c r="AU5" s="28"/>
       <c r="AV5" s="28"/>
-      <c r="AW5" s="29"/>
-      <c r="AX5" s="18"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="29"/>
       <c r="AY5" s="18"/>
-    </row>
-    <row r="6" spans="1:60" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AZ5" s="18"/>
+    </row>
+    <row r="6" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1923,273 +1950,276 @@
       <c r="W6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="X6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AD6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AE6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AI6" s="8" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AK6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AL6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AM6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AM6" s="14" t="s">
+      <c r="AN6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AP6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AQ6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AS6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AW6" s="14" t="s">
+      <c r="AX6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AX6" s="2" t="s">
+      <c r="AY6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AY6" s="4" t="s">
+      <c r="AZ6" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048575" s="13"/>
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AJ5:AM5"/>
-    <mergeCell ref="AN5:AW5"/>
-    <mergeCell ref="Z5:AI5"/>
+    <mergeCell ref="AK5:AN5"/>
+    <mergeCell ref="AO5:AX5"/>
+    <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="O5:V5"/>
-    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2500,7 +2530,11 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add Sale Ratio column to desk review workbooks (#38)
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F1241-156A-4263-93F8-102CD557789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C62BF-04D4-416B-988C-0602B5F8683A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AY$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AZ$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -50,7 +50,20 @@
     <author>Daniel F. Snow</author>
   </authors>
   <commentList>
-    <comment ref="AB6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{2D923700-2902-4CB6-8749-A7F11C03AEC1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The estimated value for the parcel (Total) divided by the amount of its most recent sale, if one exists (Sale Amount 1). Empty if no recent sales exist. If a recent sale exists but is flagged as a non-arm's-length sale, this ratio will likely not be accurate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
       <text>
         <r>
           <rPr>
@@ -64,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
+    <comment ref="AE6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
       <text>
         <r>
           <rPr>
@@ -117,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
+    <comment ref="AJ6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
       <text>
         <r>
           <rPr>
@@ -170,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
           <rPr>
@@ -183,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
@@ -197,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
       <text>
         <r>
           <rPr>
@@ -210,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -224,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -238,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -251,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -264,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -277,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -290,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -332,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>PIN</t>
   </si>
@@ -545,6 +558,9 @@
   </si>
   <si>
     <t>Min AV</t>
+  </si>
+  <si>
+    <t>Sale Ratio</t>
   </si>
 </sst>
 </file>
@@ -786,7 +802,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -906,6 +922,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -934,7 +956,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.642089004628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45351.582175115742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1569,13 +1591,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH1048575"/>
+  <dimension ref="A1:BI1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1598,30 +1620,30 @@
     <col min="19" max="19" width="11" style="10"/>
     <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
     <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
-    <col min="23" max="23" width="11" style="12"/>
-    <col min="24" max="24" width="11" style="11"/>
-    <col min="25" max="25" width="21.125" style="11" customWidth="1"/>
-    <col min="26" max="26" width="13" customWidth="1"/>
-    <col min="27" max="27" width="13" style="10" customWidth="1"/>
-    <col min="28" max="28" width="18.625" style="10" customWidth="1"/>
-    <col min="29" max="31" width="13" style="16" customWidth="1"/>
-    <col min="32" max="32" width="13" style="10" customWidth="1"/>
-    <col min="33" max="34" width="18.625" style="10" customWidth="1"/>
-    <col min="35" max="35" width="13" style="16" customWidth="1"/>
-    <col min="38" max="38" width="11" style="13"/>
-    <col min="40" max="40" width="15.625" customWidth="1"/>
-    <col min="41" max="41" width="17.375" customWidth="1"/>
-    <col min="42" max="43" width="15.625" customWidth="1"/>
-    <col min="44" max="44" width="12.625" customWidth="1"/>
-    <col min="45" max="45" width="13.25" customWidth="1"/>
-    <col min="46" max="46" width="14.125" customWidth="1"/>
-    <col min="48" max="48" width="14" customWidth="1"/>
-    <col min="49" max="49" width="14.875" customWidth="1"/>
-    <col min="50" max="50" width="11.875" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="10.875" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="11" style="12"/>
+    <col min="25" max="25" width="11" style="11"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="27" max="27" width="13" customWidth="1"/>
+    <col min="28" max="28" width="13" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="30" max="32" width="13" style="16" customWidth="1"/>
+    <col min="33" max="33" width="13" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
+    <col min="36" max="36" width="13" style="16" customWidth="1"/>
+    <col min="39" max="39" width="11" style="13"/>
+    <col min="41" max="41" width="15.625" customWidth="1"/>
+    <col min="42" max="42" width="17.375" customWidth="1"/>
+    <col min="43" max="44" width="15.625" customWidth="1"/>
+    <col min="45" max="45" width="12.625" customWidth="1"/>
+    <col min="46" max="46" width="13.25" customWidth="1"/>
+    <col min="47" max="47" width="14.125" customWidth="1"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
+    <col min="50" max="50" width="14.875" customWidth="1"/>
+    <col min="51" max="51" width="11.875" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="10.875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1682,8 +1704,9 @@
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
       <c r="BH1" s="5"/>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BI1" s="5"/>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1709,7 +1732,7 @@
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="AA2"/>
+      <c r="Z2"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
@@ -1718,9 +1741,10 @@
       <c r="AG2"/>
       <c r="AH2"/>
       <c r="AI2"/>
-      <c r="AL2"/>
-    </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AJ2"/>
+      <c r="AM2"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1747,7 +1771,7 @@
       <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
-      <c r="AA3"/>
+      <c r="Z3"/>
       <c r="AB3"/>
       <c r="AC3"/>
       <c r="AD3"/>
@@ -1756,9 +1780,10 @@
       <c r="AG3"/>
       <c r="AH3"/>
       <c r="AI3"/>
-      <c r="AL3"/>
-    </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AJ3"/>
+      <c r="AM3"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1778,7 +1803,7 @@
       <c r="W4"/>
       <c r="X4"/>
       <c r="Y4"/>
-      <c r="AA4"/>
+      <c r="Z4"/>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
@@ -1787,9 +1812,10 @@
       <c r="AG4"/>
       <c r="AH4"/>
       <c r="AI4"/>
-      <c r="AL4"/>
-    </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="AJ4"/>
+      <c r="AM4"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>50</v>
       </c>
@@ -1816,32 +1842,32 @@
       <c r="W5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="19" t="s">
+      <c r="X5" s="48"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="Z5" s="30" t="s">
+      <c r="AA5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="AA5" s="31"/>
       <c r="AB5" s="31"/>
-      <c r="AC5" s="32"/>
+      <c r="AC5" s="31"/>
       <c r="AD5" s="32"/>
-      <c r="AE5" s="31"/>
+      <c r="AE5" s="32"/>
       <c r="AF5" s="31"/>
       <c r="AG5" s="31"/>
-      <c r="AH5" s="32"/>
-      <c r="AI5" s="33"/>
-      <c r="AJ5" s="24" t="s">
+      <c r="AH5" s="31"/>
+      <c r="AI5" s="32"/>
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AK5" s="25"/>
       <c r="AL5" s="25"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="27" t="s">
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" s="28"/>
       <c r="AP5" s="28"/>
       <c r="AQ5" s="28"/>
       <c r="AR5" s="28"/>
@@ -1849,11 +1875,12 @@
       <c r="AT5" s="28"/>
       <c r="AU5" s="28"/>
       <c r="AV5" s="28"/>
-      <c r="AW5" s="29"/>
-      <c r="AX5" s="18"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="29"/>
       <c r="AY5" s="18"/>
-    </row>
-    <row r="6" spans="1:60" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AZ5" s="18"/>
+    </row>
+    <row r="6" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1923,273 +1950,276 @@
       <c r="W6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="X6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AD6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AE6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AE6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AI6" s="8" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AK6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AL6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AM6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AM6" s="14" t="s">
+      <c r="AN6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AN6" s="9" t="s">
+      <c r="AO6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AO6" s="9" t="s">
+      <c r="AP6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AP6" s="9" t="s">
+      <c r="AQ6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AQ6" s="9" t="s">
+      <c r="AR6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AS6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AW6" s="14" t="s">
+      <c r="AX6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AX6" s="2" t="s">
+      <c r="AY6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AY6" s="4" t="s">
+      <c r="AZ6" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="1048519" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="37:37" x14ac:dyDescent="0.25">
-      <c r="AK1048575" s="13"/>
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048519" s="13"/>
+    </row>
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048520" s="13"/>
+    </row>
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048521" s="13"/>
+    </row>
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048522" s="13"/>
+    </row>
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048523" s="13"/>
+    </row>
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048524" s="13"/>
+    </row>
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048525" s="13"/>
+    </row>
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048526" s="13"/>
+    </row>
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048527" s="13"/>
+    </row>
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048528" s="13"/>
+    </row>
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048529" s="13"/>
+    </row>
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048530" s="13"/>
+    </row>
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048531" s="13"/>
+    </row>
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048532" s="13"/>
+    </row>
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048533" s="13"/>
+    </row>
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048534" s="13"/>
+    </row>
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048535" s="13"/>
+    </row>
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048536" s="13"/>
+    </row>
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048537" s="13"/>
+    </row>
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048538" s="13"/>
+    </row>
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048539" s="13"/>
+    </row>
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048540" s="13"/>
+    </row>
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048541" s="13"/>
+    </row>
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048542" s="13"/>
+    </row>
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048543" s="13"/>
+    </row>
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048544" s="13"/>
+    </row>
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048545" s="13"/>
+    </row>
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048546" s="13"/>
+    </row>
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048547" s="13"/>
+    </row>
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048548" s="13"/>
+    </row>
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048549" s="13"/>
+    </row>
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048550" s="13"/>
+    </row>
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048551" s="13"/>
+    </row>
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048552" s="13"/>
+    </row>
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048553" s="13"/>
+    </row>
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048554" s="13"/>
+    </row>
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048555" s="13"/>
+    </row>
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048556" s="13"/>
+    </row>
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048557" s="13"/>
+    </row>
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048558" s="13"/>
+    </row>
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048559" s="13"/>
+    </row>
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048560" s="13"/>
+    </row>
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048561" s="13"/>
+    </row>
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048562" s="13"/>
+    </row>
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048563" s="13"/>
+    </row>
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048564" s="13"/>
+    </row>
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048565" s="13"/>
+    </row>
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048566" s="13"/>
+    </row>
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048567" s="13"/>
+    </row>
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048568" s="13"/>
+    </row>
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048569" s="13"/>
+    </row>
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048570" s="13"/>
+    </row>
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048571" s="13"/>
+    </row>
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048572" s="13"/>
+    </row>
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048573" s="13"/>
+    </row>
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
+      <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AJ5:AM5"/>
-    <mergeCell ref="AN5:AW5"/>
-    <mergeCell ref="Z5:AI5"/>
+    <mergeCell ref="AK5:AN5"/>
+    <mergeCell ref="AO5:AX5"/>
+    <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="O5:V5"/>
-    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2500,7 +2530,11 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update DR sheets to include new sales and indicators
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F1241-156A-4263-93F8-102CD557789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F77AE3-07D0-4C0A-84C3-011E4EFA316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AY$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BD$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -59,8 +59,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
-If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+          <t>Red = Non-arms-length sales
+Orange = Adjusted multi-PIN sale
+Purple = Sale added after 3/11/2024</t>
         </r>
       </text>
     </comment>
@@ -332,7 +333,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>PIN</t>
   </si>
@@ -545,6 +546,24 @@
   </si>
   <si>
     <t>Min AV</t>
+  </si>
+  <si>
+    <t>Sale 1 Added Later</t>
+  </si>
+  <si>
+    <t>Sale 2 Added Later</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>Nom. Change</t>
+  </si>
+  <si>
+    <t>Original FMV</t>
+  </si>
+  <si>
+    <t>Compared to 2024-02-16-silly-billy</t>
   </si>
 </sst>
 </file>
@@ -558,7 +577,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -617,8 +636,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +690,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,7 +818,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -905,6 +937,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -934,7 +978,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45337.642089004628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45362.554811458336" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1569,13 +1613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH1048575"/>
+  <dimension ref="A1:BM1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1616,12 +1660,13 @@
     <col min="45" max="45" width="13.25" customWidth="1"/>
     <col min="46" max="46" width="14.125" customWidth="1"/>
     <col min="48" max="48" width="14" customWidth="1"/>
-    <col min="49" max="49" width="14.875" customWidth="1"/>
-    <col min="50" max="50" width="11.875" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="10.875" hidden="1" customWidth="1"/>
+    <col min="49" max="54" width="14.875" customWidth="1"/>
+    <col min="55" max="55" width="11.875" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="10.875" hidden="1" customWidth="1"/>
+    <col min="57" max="57" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:65" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1682,8 +1727,13 @@
       <c r="BF1" s="5"/>
       <c r="BG1" s="5"/>
       <c r="BH1" s="5"/>
-    </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1720,7 +1770,7 @@
       <c r="AI2"/>
       <c r="AL2"/>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1758,7 +1808,7 @@
       <c r="AI3"/>
       <c r="AL3"/>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1789,7 +1839,7 @@
       <c r="AI4"/>
       <c r="AL4"/>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>50</v>
       </c>
@@ -1850,10 +1900,17 @@
       <c r="AU5" s="28"/>
       <c r="AV5" s="28"/>
       <c r="AW5" s="29"/>
-      <c r="AX5" s="18"/>
-      <c r="AY5" s="18"/>
-    </row>
-    <row r="6" spans="1:60" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AX5" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY5" s="50"/>
+      <c r="AZ5" s="50"/>
+      <c r="BA5" s="50"/>
+      <c r="BB5" s="51"/>
+      <c r="BC5" s="18"/>
+      <c r="BD5" s="18"/>
+    </row>
+    <row r="6" spans="1:65" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2001,10 +2058,25 @@
       <c r="AW6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AX6" s="2" t="s">
+      <c r="AX6" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY6" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ6" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA6" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB6" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AY6" s="4" t="s">
+      <c r="BD6" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2180,7 +2252,8 @@
       <c r="AK1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="AX5:BB5"/>
     <mergeCell ref="AJ5:AM5"/>
     <mergeCell ref="AN5:AW5"/>
     <mergeCell ref="Z5:AI5"/>
@@ -2500,7 +2573,11 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update training/input data (#41)
* Update CCAO package with new vars_dict

* Update input data with new sales

* Bump all renv dependencies

* Revert dependency changes

* Update CCAO package

* Add ingest kludges to support added sales

* Update DVC input data

* Include added_later indicator in DR output

* Update DR sheets to include new sales and indicators

* Update final export run ID

* Add previous values to reference cols

* Revert RP township test
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C62BF-04D4-416B-988C-0602B5F8683A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567D67E6-7F59-44CA-B726-9321EFD91864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$AZ$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BE$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="16" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,11 +46,11 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Daniel F. Snow</author>
     <author>Jean Cochrane</author>
-    <author>Daniel F. Snow</author>
   </authors>
   <commentList>
-    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{2D923700-2902-4CB6-8749-A7F11C03AEC1}">
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{E149B295-71F4-4E76-8277-523FD1D32D0E}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC6" authorId="0" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
+    <comment ref="AC6" authorId="1" shapeId="0" xr:uid="{ABE5DCF4-4803-4E6C-8CBF-CE60AF734F68}">
       <text>
         <r>
           <rPr>
@@ -72,12 +72,13 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column indicates whether this sale has been automatically flagged as a non-arm's-length sale by our sales validation algorithm.
-If the sale has been flagged, this column will contain the reason for the flag; otherwise, this column will be empty.</t>
+          <t>Red = Non-arms-length sales
+Orange = Adjusted multi-PIN sale
+Purple = Sale added after 3/11/2024</t>
         </r>
       </text>
     </comment>
-    <comment ref="AE6" authorId="1" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
+    <comment ref="AE6" authorId="0" shapeId="0" xr:uid="{1F215ACE-BB09-4EEE-A558-D6DB3D7717E6}">
       <text>
         <r>
           <rPr>
@@ -130,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ6" authorId="1" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
+    <comment ref="AJ6" authorId="0" shapeId="0" xr:uid="{CC1FC580-E9A0-4023-AFD9-5FC6F072626E}">
       <text>
         <r>
           <rPr>
@@ -183,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO6" authorId="0" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AO6" authorId="1" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
           <rPr>
@@ -196,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AP6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
@@ -210,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="0" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
+    <comment ref="AQ6" authorId="1" shapeId="0" xr:uid="{5CFDEE6F-BE90-4C3F-B1A9-702C1BFE9287}">
       <text>
         <r>
           <rPr>
@@ -223,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="0" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AR6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -237,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="0" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -251,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -264,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -277,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -290,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -303,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -345,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>PIN</t>
   </si>
@@ -558,6 +559,24 @@
   </si>
   <si>
     <t>Min AV</t>
+  </si>
+  <si>
+    <t>Sale 1 Added Later</t>
+  </si>
+  <si>
+    <t>Sale 2 Added Later</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>Nom. Change</t>
+  </si>
+  <si>
+    <t>Original FMV</t>
+  </si>
+  <si>
+    <t>Compared to 2024-02-16-silly-billy</t>
   </si>
   <si>
     <t>Sale Ratio</t>
@@ -574,7 +593,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -633,8 +652,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,6 +706,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,7 +834,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -851,42 +883,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -914,20 +910,59 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -956,11 +991,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45351.582175115742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45362.605598958333" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="51">
+  <cacheFields count="57">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1035,6 +1070,9 @@
     <cacheField name="YoY ∆ %" numFmtId="9">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
+    <cacheField name="Sale Ratio" numFmtId="9">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
     <cacheField name="Valuations Notes" numFmtId="9">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1108,6 +1146,21 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale 1 Added Later" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Sale 2 Added Later" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Original FMV" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Nom. Change" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="% Change" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1179,14 +1232,20 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="51">
+  <pivotFields count="57">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -1216,6 +1275,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1276,10 +1341,10 @@
     </i>
   </colItems>
   <dataFields count="5">
-    <dataField name="Min AV" fld="49" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV" fld="49" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max AV" fld="49" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV Difference" fld="50" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min AV" fld="55" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV" fld="55" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max AV" fld="55" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV Difference" fld="56" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1591,13 +1656,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI1048575"/>
+  <dimension ref="A1:BN1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1620,8 +1685,8 @@
     <col min="19" max="19" width="11" style="10"/>
     <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
     <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
-    <col min="23" max="24" width="11" style="12"/>
-    <col min="25" max="25" width="11" style="11"/>
+    <col min="23" max="23" width="11" style="12"/>
+    <col min="24" max="25" width="11" style="11"/>
     <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
@@ -1638,21 +1703,22 @@
     <col min="46" max="46" width="13.25" customWidth="1"/>
     <col min="47" max="47" width="14.125" customWidth="1"/>
     <col min="49" max="49" width="14" customWidth="1"/>
-    <col min="50" max="50" width="14.875" customWidth="1"/>
-    <col min="51" max="51" width="11.875" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="10.875" hidden="1" customWidth="1"/>
+    <col min="50" max="55" width="14.875" customWidth="1"/>
+    <col min="56" max="56" width="11.875" hidden="1" customWidth="1"/>
+    <col min="57" max="57" width="10.875" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1705,8 +1771,13 @@
       <c r="BG1" s="5"/>
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
-    </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1744,13 +1815,13 @@
       <c r="AJ2"/>
       <c r="AM2"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1783,7 +1854,7 @@
       <c r="AJ3"/>
       <c r="AM3"/>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1815,72 +1886,79 @@
       <c r="AJ4"/>
       <c r="AM4"/>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="44" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="45"/>
+      <c r="X5" s="50"/>
+      <c r="Y5" s="48"/>
       <c r="Z5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="AA5" s="30" t="s">
+      <c r="AA5" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="31"/>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="31"/>
-      <c r="AG5" s="31"/>
-      <c r="AH5" s="31"/>
-      <c r="AI5" s="32"/>
-      <c r="AJ5" s="33"/>
-      <c r="AK5" s="24" t="s">
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="44"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="45"/>
+      <c r="AK5" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="AL5" s="25"/>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="27" t="s">
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="38"/>
+      <c r="AO5" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="AP5" s="28"/>
-      <c r="AQ5" s="28"/>
-      <c r="AR5" s="28"/>
-      <c r="AS5" s="28"/>
-      <c r="AT5" s="28"/>
-      <c r="AU5" s="28"/>
-      <c r="AV5" s="28"/>
-      <c r="AW5" s="28"/>
-      <c r="AX5" s="29"/>
-      <c r="AY5" s="18"/>
-      <c r="AZ5" s="18"/>
-    </row>
-    <row r="6" spans="1:61" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="40"/>
+      <c r="AR5" s="40"/>
+      <c r="AS5" s="40"/>
+      <c r="AT5" s="40"/>
+      <c r="AU5" s="40"/>
+      <c r="AV5" s="40"/>
+      <c r="AW5" s="40"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ5" s="34"/>
+      <c r="BA5" s="34"/>
+      <c r="BB5" s="34"/>
+      <c r="BC5" s="35"/>
+      <c r="BD5" s="18"/>
+      <c r="BE5" s="18"/>
+    </row>
+    <row r="6" spans="1:66" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1950,11 +2028,11 @@
       <c r="W6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="49" t="s">
-        <v>71</v>
+      <c r="Y6" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>55</v>
@@ -2031,10 +2109,25 @@
       <c r="AX6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AY6" s="2" t="s">
+      <c r="AY6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="BA6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="BC6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BD6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AZ6" s="4" t="s">
+      <c r="BE6" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2210,16 +2303,17 @@
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="AY5:BC5"/>
     <mergeCell ref="AK5:AN5"/>
     <mergeCell ref="AO5:AX5"/>
     <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
+    <mergeCell ref="W5:Y5"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="O5:V5"/>
-    <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2254,14 +2348,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -2275,24 +2369,24 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="48"/>
+      <c r="L3" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="26"/>
+      <c r="M3" s="38"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2539,14 +2633,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">

</xml_diff>

<commit_message>
New desk review template
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849AEA24-C546-4710-AB0C-3A9A711A69C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D648CCB1-1A2B-469D-9846-854CFFFD1EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -46,6 +46,7 @@
   <authors>
     <author>Daniel F. Snow</author>
     <author>Jean Cochrane</author>
+    <author>Damon Major</author>
   </authors>
   <commentList>
     <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{E149B295-71F4-4E76-8277-523FD1D32D0E}">
@@ -182,6 +183,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="AO6" authorId="2" shapeId="0" xr:uid="{629BC5BE-61C7-46FF-AF42-50F2AB817841}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1-10 categorical variable based on 5 year building level sale prices.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AP6" authorId="2" shapeId="0" xr:uid="{D9623A24-EDC0-4D66-85BB-913E541D7779}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1-100 variable based on 5 year building level sale prices.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AQ6" authorId="1" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
       <text>
         <r>
@@ -300,6 +327,19 @@
           </rPr>
           <t xml:space="preserve">Indicates the estimated value for the PIN is dramatically lower than last year's value.
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AZ6" authorId="2" shapeId="0" xr:uid="{BF8F3A0F-E29F-44E5-A6CC-DDF2B0A61BB6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>For condos without sales, strata is imputed based on longitude, latitude, year built, and units.</t>
         </r>
       </text>
     </comment>
@@ -825,7 +865,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -874,59 +914,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -952,11 +941,68 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -985,11 +1031,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="45666.669970254632" createdVersion="8" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="45691.408014583336" createdVersion="8" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="57">
+  <cacheFields count="59">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1109,7 +1155,13 @@
     <cacheField name="Lnd. S. F." numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Condo Unit S. F." numFmtId="0">
+    <cacheField name="Condo Unit S. F." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Strata 1" numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Strata 2" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Condo Non-Livable Space" numFmtId="0">
@@ -1118,9 +1170,6 @@
     <cacheField name="Condo Bld. # Sales (Past 5 Years)" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Condo Potential Common Area" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
     <cacheField name="% Ownership Sum Not Equal to 1" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1140,6 +1189,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Strata is Imputed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Sale 1 Added Later" numFmtId="0">
@@ -1232,6 +1284,8 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1239,7 +1293,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="57">
+  <pivotFields count="59">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -1269,6 +1323,8 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1335,10 +1391,10 @@
     </i>
   </colItems>
   <dataFields count="5">
-    <dataField name="Min AV" fld="55" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV" fld="55" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max AV" fld="55" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV Difference" fld="56" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min AV" fld="57" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV" fld="57" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max AV" fld="57" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV Difference" fld="58" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1652,67 +1708,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AK7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AY8" sqref="AY8"/>
+      <selection pane="bottomRight" activeCell="BE12" sqref="BE12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.59765625" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" customWidth="1"/>
+    <col min="8" max="8" width="13.8984375" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.8984375" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.8984375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.09765625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.59765625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.59765625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.59765625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.8984375" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.59765625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.09765625" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.59765625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.59765625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="41" width="11" style="13"/>
-    <col min="43" max="43" width="15.625" customWidth="1"/>
-    <col min="44" max="44" width="17.375" customWidth="1"/>
-    <col min="45" max="45" width="15.625" customWidth="1"/>
-    <col min="46" max="46" width="12.625" customWidth="1"/>
-    <col min="47" max="47" width="13.25" customWidth="1"/>
-    <col min="48" max="48" width="14.125" customWidth="1"/>
+    <col min="43" max="43" width="15.59765625" customWidth="1"/>
+    <col min="44" max="44" width="17.3984375" customWidth="1"/>
+    <col min="45" max="45" width="15.59765625" customWidth="1"/>
+    <col min="46" max="46" width="12.59765625" customWidth="1"/>
+    <col min="47" max="47" width="13.19921875" customWidth="1"/>
+    <col min="48" max="48" width="14.09765625" customWidth="1"/>
     <col min="50" max="51" width="14" customWidth="1"/>
-    <col min="52" max="57" width="14.875" customWidth="1"/>
-    <col min="58" max="58" width="11.875" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="10.875" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="15.25" customWidth="1"/>
+    <col min="52" max="57" width="14.8984375" customWidth="1"/>
+    <col min="58" max="58" width="11.8984375" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="10.8984375" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1773,7 +1829,7 @@
       <c r="BO1" s="5"/>
       <c r="BP1" s="5"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1813,13 +1869,13 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1854,7 +1910,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1888,81 +1944,81 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="B5" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="39" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="41"/>
+      <c r="X5" s="51"/>
+      <c r="Y5" s="52"/>
       <c r="Z5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="AA5" s="33" t="s">
+      <c r="AA5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="35"/>
-      <c r="AE5" s="35"/>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="34"/>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="35"/>
-      <c r="AJ5" s="36"/>
-      <c r="AK5" s="27" t="s">
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="AL5" s="28"/>
-      <c r="AM5" s="28"/>
-      <c r="AN5" s="28"/>
-      <c r="AO5" s="28"/>
-      <c r="AP5" s="29"/>
-      <c r="AQ5" s="30" t="s">
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="38"/>
+      <c r="AO5" s="37"/>
+      <c r="AP5" s="39"/>
+      <c r="AQ5" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="AR5" s="31"/>
-      <c r="AS5" s="31"/>
-      <c r="AT5" s="31"/>
-      <c r="AU5" s="31"/>
-      <c r="AV5" s="31"/>
-      <c r="AW5" s="31"/>
-      <c r="AX5" s="31"/>
-      <c r="AY5" s="31"/>
-      <c r="AZ5" s="32"/>
-      <c r="BA5" s="24" t="s">
+      <c r="AR5" s="41"/>
+      <c r="AS5" s="41"/>
+      <c r="AT5" s="41"/>
+      <c r="AU5" s="41"/>
+      <c r="AV5" s="41"/>
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="43"/>
+      <c r="BA5" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="BB5" s="25"/>
-      <c r="BC5" s="25"/>
-      <c r="BD5" s="25"/>
-      <c r="BE5" s="26"/>
+      <c r="BB5" s="34"/>
+      <c r="BC5" s="34"/>
+      <c r="BD5" s="34"/>
+      <c r="BE5" s="35"/>
       <c r="BF5" s="18"/>
       <c r="BG5" s="18"/>
     </row>
-    <row r="6" spans="1:68" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2112,7 @@
       <c r="AE6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AF6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="AG6" s="3" t="s">
@@ -2068,7 +2124,7 @@
       <c r="AI6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AJ6" s="8" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>64</v>
       </c>
       <c r="AK6" s="3" t="s">
@@ -2080,13 +2136,13 @@
       <c r="AM6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AN6" s="14" t="s">
+      <c r="AN6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="AO6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AP6" s="51" t="s">
+      <c r="AP6" s="24" t="s">
         <v>78</v>
       </c>
       <c r="AQ6" s="9" t="s">
@@ -2113,10 +2169,10 @@
       <c r="AX6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AY6" s="14" t="s">
+      <c r="AY6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AZ6" s="51" t="s">
+      <c r="AZ6" s="24" t="s">
         <v>79</v>
       </c>
       <c r="BA6" s="9" t="s">
@@ -2131,7 +2187,7 @@
       <c r="BD6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BE6" s="14" t="s">
         <v>72</v>
       </c>
       <c r="BF6" s="2" t="s">
@@ -2141,175 +2197,175 @@
         <v>62</v>
       </c>
     </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.3">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
@@ -2342,63 +2398,63 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="42.625" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" customWidth="1"/>
+    <col min="3" max="3" width="42.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" customWidth="1"/>
+    <col min="5" max="6" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.8984375" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.375" customWidth="1"/>
+    <col min="13" max="13" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+      <c r="B1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="27" t="s">
+      <c r="K3" s="52"/>
+      <c r="L3" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="29"/>
-    </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="M3" s="39"/>
+    </row>
+    <row r="4" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2439,175 +2495,175 @@
         <v>44</v>
       </c>
     </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2631,28 +2687,28 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="B1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>58</v>
       </c>
@@ -2672,7 +2728,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>59</v>
       </c>
@@ -2682,7 +2738,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Update Desk Review template
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA15CA4-7597-4D8E-A3A5-12992E07131D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DD87FD-E237-4D77-B894-A07235D10A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="4872" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BB$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BA$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -192,7 +192,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1-10 variable based on 5 year building level sale prices.</t>
+          <t xml:space="preserve">This is the 5-year, time-weighted, rolling average of building sale prices </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>excluding the current sale.</t>
         </r>
       </text>
     </comment>
@@ -205,7 +215,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1-100 variable based on 5 year building level sale prices.</t>
+          <t>This is the count of the sales used to make the building sale average.</t>
         </r>
       </text>
     </comment>
@@ -330,19 +340,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="2" shapeId="0" xr:uid="{BF8F3A0F-E29F-44E5-A6CC-DDF2B0A61BB6}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>For condos without sales, strata is imputed based on longitude, latitude, year built, and number of units.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -371,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>PIN</t>
   </si>
@@ -586,13 +583,10 @@
     <t>Sale Ratio</t>
   </si>
   <si>
-    <t>Strata 1</t>
-  </si>
-  <si>
-    <t>Strata 2</t>
-  </si>
-  <si>
-    <t>Strata is Imputed</t>
+    <t>Building Sale Avg.</t>
+  </si>
+  <si>
+    <t>Building Sale Cnt.</t>
   </si>
 </sst>
 </file>
@@ -834,7 +828,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -883,9 +877,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -893,9 +884,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -991,7 +979,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="45691.466369907408" createdVersion="8" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45693.469423032409" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1231,7 +1219,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="54">
     <pivotField showAll="0"/>
@@ -1641,69 +1629,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK1048575"/>
+  <dimension ref="A1:BJ1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AK7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="BD13" sqref="BD13"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.59765625" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" customWidth="1"/>
-    <col min="8" max="8" width="13.8984375" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.8984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.8984375" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.09765625" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.59765625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.59765625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.59765625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.8984375" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.59765625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.09765625" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.59765625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.59765625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
-    <col min="39" max="41" width="11" style="13"/>
-    <col min="43" max="43" width="15.59765625" customWidth="1"/>
-    <col min="44" max="44" width="17.3984375" customWidth="1"/>
-    <col min="45" max="45" width="15.59765625" customWidth="1"/>
-    <col min="46" max="46" width="12.59765625" customWidth="1"/>
-    <col min="47" max="47" width="13.19921875" customWidth="1"/>
-    <col min="48" max="48" width="14.09765625" customWidth="1"/>
+    <col min="39" max="40" width="11" style="13"/>
+    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="16.625" customWidth="1"/>
+    <col min="43" max="43" width="15.625" customWidth="1"/>
+    <col min="44" max="44" width="17.375" customWidth="1"/>
+    <col min="45" max="45" width="15.625" customWidth="1"/>
+    <col min="46" max="46" width="12.625" customWidth="1"/>
+    <col min="47" max="47" width="13.25" customWidth="1"/>
+    <col min="48" max="48" width="14.125" customWidth="1"/>
     <col min="50" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="14.8984375" customWidth="1"/>
-    <col min="53" max="53" width="9.3984375" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="9.8984375" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="15.19921875" customWidth="1"/>
+    <col min="52" max="52" width="9.375" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="9.875" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1757,9 +1746,8 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-      <c r="BK1" s="5"/>
-    </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1799,13 +1787,13 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1840,7 +1828,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1874,74 +1862,73 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="35" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="X5" s="36"/>
-      <c r="Y5" s="37"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="35"/>
       <c r="Z5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="AA5" s="29" t="s">
+      <c r="AA5" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="30"/>
-      <c r="AI5" s="31"/>
-      <c r="AJ5" s="32"/>
-      <c r="AK5" s="46" t="s">
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="28"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="30"/>
+      <c r="AK5" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AL5" s="47"/>
-      <c r="AM5" s="47"/>
-      <c r="AN5" s="48"/>
-      <c r="AO5" s="47"/>
-      <c r="AP5" s="49"/>
-      <c r="AQ5" s="25" t="s">
+      <c r="AL5" s="45"/>
+      <c r="AM5" s="45"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="45"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="AR5" s="26"/>
-      <c r="AS5" s="26"/>
-      <c r="AT5" s="26"/>
-      <c r="AU5" s="26"/>
-      <c r="AV5" s="26"/>
-      <c r="AW5" s="26"/>
-      <c r="AX5" s="26"/>
-      <c r="AY5" s="27"/>
-      <c r="AZ5" s="28"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="25"/>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
+      <c r="AW5" s="25"/>
+      <c r="AX5" s="25"/>
+      <c r="AY5" s="26"/>
+      <c r="AZ5" s="18"/>
       <c r="BA5" s="18"/>
-      <c r="BB5" s="18"/>
-    </row>
-    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:62" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2065,7 +2052,7 @@
       <c r="AO6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AP6" s="24" t="s">
+      <c r="AP6" s="14" t="s">
         <v>72</v>
       </c>
       <c r="AQ6" s="9" t="s">
@@ -2095,190 +2082,187 @@
       <c r="AY6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AZ6" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="BA6" s="2" t="s">
+      <c r="AZ6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BB6" s="4" t="s">
+      <c r="BA6" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.3">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AQ5:AZ5"/>
+    <mergeCell ref="AQ5:AY5"/>
     <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="W5:Y5"/>
@@ -2302,66 +2286,66 @@
       <pane xSplit="1" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" customWidth="1"/>
-    <col min="2" max="2" width="7.69921875" customWidth="1"/>
-    <col min="3" max="3" width="42.59765625" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" customWidth="1"/>
-    <col min="5" max="6" width="11.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.8984375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.3984375" customWidth="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="50" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="46" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="49"/>
-    </row>
-    <row r="4" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="M3" s="47"/>
+    </row>
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2402,175 +2386,175 @@
         <v>44</v>
       </c>
     </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2591,31 +2575,38 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" activeRow="4" previousRow="4" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+          <references count="1">
+            <reference field="2" count="0"/>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>58</v>
       </c>
@@ -2635,7 +2626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>59</v>
       </c>
@@ -2645,7 +2636,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Add flag for imputed bldg mean
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfsnow/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DD87FD-E237-4D77-B894-A07235D10A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC8075B-C40E-F245-B474-80C27F1FA2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42560" windowHeight="23440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BA$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BB$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -188,7 +188,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -198,7 +198,7 @@
           <rPr>
             <i/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -211,7 +211,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -219,12 +219,25 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="1" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AQ6" authorId="1" shapeId="0" xr:uid="{A8C86961-FCD8-2D46-9B65-1771893FF3A6}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the building-level rolling average column (shown to the left) was imputed, as there were not sufficient sales in the building.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AR6" authorId="1" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -232,12 +245,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -246,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -260,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -274,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -287,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -300,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -313,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -326,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AZ6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -368,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>PIN</t>
   </si>
@@ -583,10 +596,13 @@
     <t>Sale Ratio</t>
   </si>
   <si>
-    <t>Building Sale Avg.</t>
-  </si>
-  <si>
-    <t>Building Sale Cnt.</t>
+    <t>Bldg. Sale Avg.</t>
+  </si>
+  <si>
+    <t>Bldg. Sale Cnt.</t>
+  </si>
+  <si>
+    <t>Bldg. Sale Avg. was Imputed</t>
   </si>
 </sst>
 </file>
@@ -600,7 +616,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -656,6 +672,19 @@
       <i/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -979,11 +1008,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45693.469423032409" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Dan Snow" refreshedDate="45698.539430555553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="54">
+  <cacheFields count="53">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1106,10 +1135,10 @@
     <cacheField name="Condo Unit S. F." numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Strata 1" numFmtId="37">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Strata 2" numFmtId="0">
+    <cacheField name="Building Sale Avg." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building Sale Cnt." numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Condo Non-Livable Space" numFmtId="0">
@@ -1137,9 +1166,6 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Strata is Imputed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1213,15 +1239,14 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="54">
+  <pivotFields count="53">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -1251,7 +1276,6 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1314,10 +1338,10 @@
     </i>
   </colItems>
   <dataFields count="5">
-    <dataField name="Min AV" fld="52" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV" fld="52" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max AV" fld="52" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV Difference" fld="53" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min AV" fld="51" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV" fld="51" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max AV" fld="51" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV Difference" fld="52" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1333,9 +1357,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1373,7 +1397,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1479,7 +1503,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1621,7 +1645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1629,7 +1653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ1048575"/>
+  <dimension ref="A1:BK1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -1638,52 +1662,52 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.6640625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.83203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.1640625" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.6640625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="16.625" customWidth="1"/>
-    <col min="43" max="43" width="15.625" customWidth="1"/>
-    <col min="44" max="44" width="17.375" customWidth="1"/>
-    <col min="45" max="45" width="15.625" customWidth="1"/>
-    <col min="46" max="46" width="12.625" customWidth="1"/>
-    <col min="47" max="47" width="13.25" customWidth="1"/>
-    <col min="48" max="48" width="14.125" customWidth="1"/>
-    <col min="50" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="9.375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="9.875" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="15.25" customWidth="1"/>
+    <col min="41" max="41" width="16.6640625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="16.6640625" customWidth="1"/>
+    <col min="43" max="44" width="15.6640625" customWidth="1"/>
+    <col min="45" max="45" width="17.33203125" customWidth="1"/>
+    <col min="46" max="46" width="15.6640625" customWidth="1"/>
+    <col min="47" max="47" width="12.6640625" customWidth="1"/>
+    <col min="48" max="48" width="13.1640625" customWidth="1"/>
+    <col min="49" max="49" width="14.1640625" customWidth="1"/>
+    <col min="51" max="52" width="14" customWidth="1"/>
+    <col min="53" max="53" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="9.83203125" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1746,8 +1770,9 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK1" s="5"/>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1787,7 +1812,7 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1828,7 +1853,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1862,7 +1887,7 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B5" s="31" t="s">
         <v>49</v>
       </c>
@@ -1924,11 +1949,12 @@
       <c r="AV5" s="25"/>
       <c r="AW5" s="25"/>
       <c r="AX5" s="25"/>
-      <c r="AY5" s="26"/>
-      <c r="AZ5" s="18"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="26"/>
       <c r="BA5" s="18"/>
-    </row>
-    <row r="6" spans="1:62" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BB5" s="18"/>
+    </row>
+    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2056,213 +2082,216 @@
         <v>72</v>
       </c>
       <c r="AQ6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AS6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AY6" s="8" t="s">
+      <c r="AZ6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AZ6" s="2" t="s">
+      <c r="BA6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA6" s="4" t="s">
+      <c r="BB6" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AQ5:AY5"/>
+    <mergeCell ref="AQ5:AZ5"/>
     <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="W5:Y5"/>
@@ -2289,22 +2318,22 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="42.625" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.375" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>45</v>
       </c>
@@ -2318,14 +2347,14 @@
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="48" t="s">
         <v>49</v>
       </c>
@@ -2345,7 +2374,7 @@
       </c>
       <c r="M3" s="47"/>
     </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2386,175 +2415,175 @@
         <v>44</v>
       </c>
     </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2576,27 +2605,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
-      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" activeRow="4" previousRow="4" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="2" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>57</v>
       </c>
@@ -2606,7 +2628,7 @@
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>58</v>
       </c>
@@ -2626,7 +2648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>59</v>
       </c>
@@ -2636,7 +2658,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Update params and add flag for imputed bldg mean (#103)
* Update default hyperparameters with results of CV run

Run ID: 2025-02-08-youthful-carly

* Drop daily highway traffic feature

* Add flag for imputed bldg mean
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfsnow/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DD87FD-E237-4D77-B894-A07235D10A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC8075B-C40E-F245-B474-80C27F1FA2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42560" windowHeight="23440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BA$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BB$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -188,7 +188,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -198,7 +198,7 @@
           <rPr>
             <i/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -211,7 +211,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -219,12 +219,25 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ6" authorId="1" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+    <comment ref="AQ6" authorId="1" shapeId="0" xr:uid="{A8C86961-FCD8-2D46-9B65-1771893FF3A6}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates that the building-level rolling average column (shown to the left) was imputed, as there were not sufficient sales in the building.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AR6" authorId="1" shapeId="0" xr:uid="{FB860205-06EB-4D59-87E1-3924046864DA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -232,12 +245,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
+    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -246,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -260,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -274,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -287,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -300,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -313,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -326,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AZ6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -368,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>PIN</t>
   </si>
@@ -583,10 +596,13 @@
     <t>Sale Ratio</t>
   </si>
   <si>
-    <t>Building Sale Avg.</t>
-  </si>
-  <si>
-    <t>Building Sale Cnt.</t>
+    <t>Bldg. Sale Avg.</t>
+  </si>
+  <si>
+    <t>Bldg. Sale Cnt.</t>
+  </si>
+  <si>
+    <t>Bldg. Sale Avg. was Imputed</t>
   </si>
 </sst>
 </file>
@@ -600,7 +616,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -656,6 +672,19 @@
       <i/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -979,11 +1008,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45693.469423032409" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Dan Snow" refreshedDate="45698.539430555553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="54">
+  <cacheFields count="53">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1106,10 +1135,10 @@
     <cacheField name="Condo Unit S. F." numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Strata 1" numFmtId="37">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Strata 2" numFmtId="0">
+    <cacheField name="Building Sale Avg." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Building Sale Cnt." numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Condo Non-Livable Space" numFmtId="0">
@@ -1137,9 +1166,6 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Strata is Imputed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1213,15 +1239,14 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="54">
+  <pivotFields count="53">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -1251,7 +1276,6 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1314,10 +1338,10 @@
     </i>
   </colItems>
   <dataFields count="5">
-    <dataField name="Min AV" fld="52" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV" fld="52" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max AV" fld="52" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV Difference" fld="53" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min AV" fld="51" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV" fld="51" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max AV" fld="51" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average AV Difference" fld="52" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1333,9 +1357,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1373,7 +1397,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1479,7 +1503,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1621,7 +1645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1629,7 +1653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ1048575"/>
+  <dimension ref="A1:BK1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -1638,52 +1662,52 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.6640625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.83203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.1640625" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.6640625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="16.625" customWidth="1"/>
-    <col min="43" max="43" width="15.625" customWidth="1"/>
-    <col min="44" max="44" width="17.375" customWidth="1"/>
-    <col min="45" max="45" width="15.625" customWidth="1"/>
-    <col min="46" max="46" width="12.625" customWidth="1"/>
-    <col min="47" max="47" width="13.25" customWidth="1"/>
-    <col min="48" max="48" width="14.125" customWidth="1"/>
-    <col min="50" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="9.375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="9.875" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="15.25" customWidth="1"/>
+    <col min="41" max="41" width="16.6640625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="16.6640625" customWidth="1"/>
+    <col min="43" max="44" width="15.6640625" customWidth="1"/>
+    <col min="45" max="45" width="17.33203125" customWidth="1"/>
+    <col min="46" max="46" width="15.6640625" customWidth="1"/>
+    <col min="47" max="47" width="12.6640625" customWidth="1"/>
+    <col min="48" max="48" width="13.1640625" customWidth="1"/>
+    <col min="49" max="49" width="14.1640625" customWidth="1"/>
+    <col min="51" max="52" width="14" customWidth="1"/>
+    <col min="53" max="53" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="9.83203125" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1746,8 +1770,9 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK1" s="5"/>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1787,7 +1812,7 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1828,7 +1853,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1862,7 +1887,7 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
       <c r="B5" s="31" t="s">
         <v>49</v>
       </c>
@@ -1924,11 +1949,12 @@
       <c r="AV5" s="25"/>
       <c r="AW5" s="25"/>
       <c r="AX5" s="25"/>
-      <c r="AY5" s="26"/>
-      <c r="AZ5" s="18"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="26"/>
       <c r="BA5" s="18"/>
-    </row>
-    <row r="6" spans="1:62" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BB5" s="18"/>
+    </row>
+    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2056,213 +2082,216 @@
         <v>72</v>
       </c>
       <c r="AQ6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AR6" s="9" t="s">
+      <c r="AS6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AS6" s="9" t="s">
+      <c r="AT6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AT6" s="9" t="s">
+      <c r="AU6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AU6" s="9" t="s">
+      <c r="AV6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AV6" s="9" t="s">
+      <c r="AW6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AW6" s="9" t="s">
+      <c r="AX6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AX6" s="9" t="s">
+      <c r="AY6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AY6" s="8" t="s">
+      <c r="AZ6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AZ6" s="2" t="s">
+      <c r="BA6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BA6" s="4" t="s">
+      <c r="BB6" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.2">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AQ5:AY5"/>
+    <mergeCell ref="AQ5:AZ5"/>
     <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="W5:Y5"/>
@@ -2289,22 +2318,22 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="42.625" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.375" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>45</v>
       </c>
@@ -2318,14 +2347,14 @@
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="48" t="s">
         <v>49</v>
       </c>
@@ -2345,7 +2374,7 @@
       </c>
       <c r="M3" s="47"/>
     </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2386,175 +2415,175 @@
         <v>44</v>
       </c>
     </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2576,27 +2605,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
-      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" activeRow="4" previousRow="4" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="2" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>57</v>
       </c>
@@ -2606,7 +2628,7 @@
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>58</v>
       </c>
@@ -2626,7 +2648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>59</v>
       </c>
@@ -2636,7 +2658,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Drop OG 5 year sale count column. Fix formatting
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfsnow/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC8075B-C40E-F245-B474-80C27F1FA2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52830C5-95F1-408E-B5E5-E028C81A388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="42560" windowHeight="23440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BB$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BA$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -192,17 +192,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">This is the 5-year, time-weighted, rolling average of building sale prices </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>excluding the current sale.</t>
+          <t>Average of sales in the same building within the last 5 years, weighted by time</t>
         </r>
       </text>
     </comment>
@@ -215,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This is the count of the sales used to make the building sale average.</t>
+          <t>Count of sales in the same building in the last 5 years. This is the number of sales included in the average (on col to the left)</t>
         </r>
       </text>
     </comment>
@@ -245,21 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Number of sales in the building containing this PIN in the past five years.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -273,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -287,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -300,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -313,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -326,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -339,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -381,7 +357,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>PIN</t>
   </si>
@@ -482,9 +458,6 @@
     <t>Condo Unit S. F.</t>
   </si>
   <si>
-    <t>Condo Bld. # Sales (Past 5 Years)</t>
-  </si>
-  <si>
     <t>Condo Building ID (PIN10)</t>
   </si>
   <si>
@@ -596,13 +569,13 @@
     <t>Sale Ratio</t>
   </si>
   <si>
-    <t>Bldg. Sale Avg.</t>
-  </si>
-  <si>
-    <t>Bldg. Sale Cnt.</t>
-  </si>
-  <si>
     <t>Bldg. Sale Avg. was Imputed</t>
+  </si>
+  <si>
+    <t>5-Year Bldg. Sale Price Avg.</t>
+  </si>
+  <si>
+    <t>5-Year Bldg. Sale Count</t>
   </si>
 </sst>
 </file>
@@ -616,7 +589,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -676,13 +649,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -1008,7 +974,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Dan Snow" refreshedDate="45698.539430555553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45699.681777430553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1135,16 +1101,16 @@
     <cacheField name="Condo Unit S. F." numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Building Sale Avg." numFmtId="37">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Building Sale Cnt." numFmtId="0">
+    <cacheField name="Bldg. Sale Avg." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bldg. Sale Cnt." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bldg. Sale Avg. was Imputed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Condo Non-Livable Space" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Condo Bld. # Sales (Past 5 Years)" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="% Ownership Sum Not Equal to 1" numFmtId="0">
@@ -1244,7 +1210,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="53">
     <pivotField showAll="0"/>
@@ -1357,9 +1323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1397,7 +1363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1503,7 +1469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1645,7 +1611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1653,7 +1619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK1048575"/>
+  <dimension ref="A1:BJ1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
@@ -1662,52 +1628,50 @@
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.6640625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.83203125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.1640625" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.6640625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="16.6640625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="16.6640625" customWidth="1"/>
-    <col min="43" max="44" width="15.6640625" customWidth="1"/>
-    <col min="45" max="45" width="17.33203125" customWidth="1"/>
-    <col min="46" max="46" width="15.6640625" customWidth="1"/>
-    <col min="47" max="47" width="12.6640625" customWidth="1"/>
-    <col min="48" max="48" width="13.1640625" customWidth="1"/>
-    <col min="49" max="49" width="14.1640625" customWidth="1"/>
-    <col min="51" max="52" width="14" customWidth="1"/>
-    <col min="53" max="53" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="9.83203125" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="15.1640625" customWidth="1"/>
+    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="12.875" customWidth="1"/>
+    <col min="43" max="45" width="15.625" customWidth="1"/>
+    <col min="46" max="46" width="12.625" customWidth="1"/>
+    <col min="47" max="47" width="13.125" customWidth="1"/>
+    <col min="48" max="48" width="14.125" customWidth="1"/>
+    <col min="50" max="51" width="14" customWidth="1"/>
+    <col min="52" max="52" width="9.375" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="9.875" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1770,9 +1734,8 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-      <c r="BK1" s="5"/>
-    </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1812,7 +1775,7 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1853,7 +1816,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1887,9 +1850,9 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -1912,15 +1875,15 @@
       <c r="U5" s="42"/>
       <c r="V5" s="43"/>
       <c r="W5" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X5" s="34"/>
       <c r="Y5" s="35"/>
       <c r="Z5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA5" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
@@ -1932,7 +1895,7 @@
       <c r="AI5" s="29"/>
       <c r="AJ5" s="30"/>
       <c r="AK5" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AL5" s="45"/>
       <c r="AM5" s="45"/>
@@ -1940,7 +1903,7 @@
       <c r="AO5" s="45"/>
       <c r="AP5" s="47"/>
       <c r="AQ5" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
@@ -1949,12 +1912,11 @@
       <c r="AV5" s="25"/>
       <c r="AW5" s="25"/>
       <c r="AX5" s="25"/>
-      <c r="AY5" s="25"/>
-      <c r="AZ5" s="26"/>
+      <c r="AY5" s="26"/>
+      <c r="AZ5" s="18"/>
       <c r="BA5" s="18"/>
-      <c r="BB5" s="18"/>
-    </row>
-    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:62" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1971,13 +1933,13 @@
         <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>4</v>
@@ -1992,7 +1954,7 @@
         <v>24</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>7</v>
@@ -2016,7 +1978,7 @@
         <v>13</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>6</v>
@@ -2028,10 +1990,10 @@
         <v>3</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA6" s="2" t="s">
         <v>14</v>
@@ -2040,13 +2002,13 @@
         <v>15</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AF6" s="3" t="s">
         <v>17</v>
@@ -2055,13 +2017,13 @@
         <v>18</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AI6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AJ6" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AK6" s="3" t="s">
         <v>27</v>
@@ -2082,216 +2044,213 @@
         <v>72</v>
       </c>
       <c r="AQ6" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AR6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="AS6" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AT6" s="9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AU6" s="9" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="AV6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AW6" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="AX6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AZ6" s="8" t="s">
+      <c r="AY6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="BA6" s="2" t="s">
+      <c r="AZ6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BA6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BB6" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AQ5:AZ5"/>
+    <mergeCell ref="AQ5:AY5"/>
     <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="W5:Y5"/>
@@ -2318,24 +2277,24 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.83203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2347,16 +2306,16 @@
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -2366,17 +2325,17 @@
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
       <c r="J3" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="35"/>
       <c r="L3" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M3" s="47"/>
     </row>
-    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
@@ -2388,19 +2347,19 @@
         <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -2412,178 +2371,178 @@
         <v>27</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2607,20 +2566,20 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2628,29 +2587,29 @@
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>59</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -2658,9 +2617,9 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>

</xml_diff>

<commit_message>
Add flag to desk review workbook for assessable permit in past 3 years
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfsnow\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52830C5-95F1-408E-B5E5-E028C81A388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1455155-E707-422A-AE82-4E35DDC6E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,11 @@
     <sheet name="Neighborhood Breakout" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BA$7</definedName>
+    <definedName name="pin_detail_range">'PIN Detail'!$A$6:$BB$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -329,6 +329,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="AZ6" authorId="1" shapeId="0" xr:uid="{86B2F11E-7E98-4F33-84E9-503652FA11AA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Flag indicating that the PIN has at least one assessable permit in the past 3 years. Only counts permits prior to January 1st of the current assessment year.
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -357,7 +371,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>PIN</t>
   </si>
@@ -576,6 +590,9 @@
   </si>
   <si>
     <t>5-Year Bldg. Sale Count</t>
+  </si>
+  <si>
+    <t>Recent Assessable Permit</t>
   </si>
 </sst>
 </file>
@@ -589,7 +606,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -654,6 +671,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -705,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -816,6 +839,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -823,7 +855,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -945,6 +977,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -974,7 +1012,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel F. Snow" refreshedDate="45699.681777430553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.714398958335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1101,10 +1139,10 @@
     <cacheField name="Condo Unit S. F." numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Bldg. Sale Avg." numFmtId="37">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Bldg. Sale Cnt." numFmtId="0">
+    <cacheField name="5-Year Bldg. Sale Price Avg." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="5-Year Bldg. Sale Count" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Bldg. Sale Avg. was Imputed" numFmtId="0">
@@ -1210,7 +1248,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="53">
     <pivotField showAll="0"/>
@@ -1323,9 +1361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1363,7 +1401,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1469,7 +1507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1611,7 +1649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1619,13 +1657,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ1048575"/>
+  <dimension ref="A1:BK1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1666,12 +1704,13 @@
     <col min="47" max="47" width="13.125" customWidth="1"/>
     <col min="48" max="48" width="14.125" customWidth="1"/>
     <col min="50" max="51" width="14" customWidth="1"/>
-    <col min="52" max="52" width="9.375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="9.875" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="15.125" customWidth="1"/>
+    <col min="52" max="52" width="13" customWidth="1"/>
+    <col min="53" max="53" width="7.75" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="9.375" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1734,8 +1773,9 @@
       <c r="BH1" s="5"/>
       <c r="BI1" s="5"/>
       <c r="BJ1" s="5"/>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK1" s="5"/>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1775,7 +1815,7 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1816,7 +1856,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1850,7 +1890,7 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
         <v>48</v>
       </c>
@@ -1913,10 +1953,11 @@
       <c r="AW5" s="25"/>
       <c r="AX5" s="25"/>
       <c r="AY5" s="26"/>
-      <c r="AZ5" s="18"/>
+      <c r="AZ5" s="50"/>
       <c r="BA5" s="18"/>
-    </row>
-    <row r="6" spans="1:62" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BB5" s="18"/>
+    </row>
+    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2070,10 +2111,13 @@
       <c r="AY6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AZ6" s="2" t="s">
+      <c r="AZ6" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="BA6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BA6" s="4" t="s">
+      <c r="BB6" s="4" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add flag to desk review workbook for assessable permit in past 3 years (#104)
* Drop OG 5 year sale count column. Fix formatting

* Set final model for export

* Add flag to desk review workbook for assessable permit in past 3 years

---------

Co-authored-by: Dan Snow <daniel.snow@cookcountyil.gov>
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfsnow/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC8075B-C40E-F245-B474-80C27F1FA2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1455155-E707-422A-AE82-4E35DDC6E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="42560" windowHeight="23440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -192,17 +192,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">This is the 5-year, time-weighted, rolling average of building sale prices </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>excluding the current sale.</t>
+          <t>Average of sales in the same building within the last 5 years, weighted by time</t>
         </r>
       </text>
     </comment>
@@ -215,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This is the count of the sales used to make the building sale average.</t>
+          <t>Count of sales in the same building in the last 5 years. This is the number of sales included in the average (on col to the left)</t>
         </r>
       </text>
     </comment>
@@ -245,21 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{DE66952B-3B78-41CA-8F95-BEB0CF94AFE3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Number of sales in the building containing this PIN in the past five years.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
+    <comment ref="AS6" authorId="1" shapeId="0" xr:uid="{19EE9F95-A56E-4EA0-9134-F06506AB7CBD}">
       <text>
         <r>
           <rPr>
@@ -273,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
+    <comment ref="AT6" authorId="1" shapeId="0" xr:uid="{639FF332-651B-4102-84EB-A672D45FE5DD}">
       <text>
         <r>
           <rPr>
@@ -287,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
+    <comment ref="AU6" authorId="1" shapeId="0" xr:uid="{6740D397-A648-4E6F-9B93-3CD31DC6D8BA}">
       <text>
         <r>
           <rPr>
@@ -300,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
+    <comment ref="AV6" authorId="1" shapeId="0" xr:uid="{7D040200-0E0F-46B6-9198-8C69CBBCC045}">
       <text>
         <r>
           <rPr>
@@ -313,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
+    <comment ref="AW6" authorId="1" shapeId="0" xr:uid="{24A573B4-21BB-4433-A2C7-BA31FACE2B8B}">
       <text>
         <r>
           <rPr>
@@ -326,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
+    <comment ref="AX6" authorId="1" shapeId="0" xr:uid="{3971B04C-87F5-436E-BE63-1FC23AE80FEF}">
       <text>
         <r>
           <rPr>
@@ -339,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
+    <comment ref="AY6" authorId="1" shapeId="0" xr:uid="{9AD145C6-4D3D-45FB-840D-6860003435DE}">
       <text>
         <r>
           <rPr>
@@ -349,6 +325,20 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Indicates the estimated value for the PIN is dramatically lower than last year's value.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AZ6" authorId="1" shapeId="0" xr:uid="{86B2F11E-7E98-4F33-84E9-503652FA11AA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Flag indicating that the PIN has at least one assessable permit in the past 3 years. Only counts permits prior to January 1st of the current assessment year.
 </t>
         </r>
       </text>
@@ -482,9 +472,6 @@
     <t>Condo Unit S. F.</t>
   </si>
   <si>
-    <t>Condo Bld. # Sales (Past 5 Years)</t>
-  </si>
-  <si>
     <t>Condo Building ID (PIN10)</t>
   </si>
   <si>
@@ -596,13 +583,16 @@
     <t>Sale Ratio</t>
   </si>
   <si>
-    <t>Bldg. Sale Avg.</t>
-  </si>
-  <si>
-    <t>Bldg. Sale Cnt.</t>
-  </si>
-  <si>
     <t>Bldg. Sale Avg. was Imputed</t>
+  </si>
+  <si>
+    <t>5-Year Bldg. Sale Price Avg.</t>
+  </si>
+  <si>
+    <t>5-Year Bldg. Sale Count</t>
+  </si>
+  <si>
+    <t>Recent Assessable Permit</t>
   </si>
 </sst>
 </file>
@@ -682,11 +672,10 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="9"/>
-      <color rgb="FF000000"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -739,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -850,6 +839,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -857,7 +855,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -979,6 +977,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1008,7 +1012,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Dan Snow" refreshedDate="45698.539430555553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.714398958335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1135,16 +1139,16 @@
     <cacheField name="Condo Unit S. F." numFmtId="37">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="Building Sale Avg." numFmtId="37">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Building Sale Cnt." numFmtId="0">
+    <cacheField name="5-Year Bldg. Sale Price Avg." numFmtId="37">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="5-Year Bldg. Sale Count" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Bldg. Sale Avg. was Imputed" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Condo Non-Livable Space" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Condo Bld. # Sales (Past 5 Years)" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="% Ownership Sum Not Equal to 1" numFmtId="0">
@@ -1659,55 +1663,54 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.6640625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.83203125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.1640625" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.6640625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="16.6640625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="16.6640625" customWidth="1"/>
-    <col min="43" max="44" width="15.6640625" customWidth="1"/>
-    <col min="45" max="45" width="17.33203125" customWidth="1"/>
-    <col min="46" max="46" width="15.6640625" customWidth="1"/>
-    <col min="47" max="47" width="12.6640625" customWidth="1"/>
-    <col min="48" max="48" width="13.1640625" customWidth="1"/>
-    <col min="49" max="49" width="14.1640625" customWidth="1"/>
-    <col min="51" max="52" width="14" customWidth="1"/>
-    <col min="53" max="53" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="9.83203125" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="15.1640625" customWidth="1"/>
+    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="12.875" customWidth="1"/>
+    <col min="43" max="45" width="15.625" customWidth="1"/>
+    <col min="46" max="46" width="12.625" customWidth="1"/>
+    <col min="47" max="47" width="13.125" customWidth="1"/>
+    <col min="48" max="48" width="14.125" customWidth="1"/>
+    <col min="50" max="51" width="14" customWidth="1"/>
+    <col min="52" max="52" width="13" customWidth="1"/>
+    <col min="53" max="53" width="7.75" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="9.375" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1772,7 +1775,7 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1812,7 +1815,7 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1853,7 +1856,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1887,9 +1890,9 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -1912,15 +1915,15 @@
       <c r="U5" s="42"/>
       <c r="V5" s="43"/>
       <c r="W5" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X5" s="34"/>
       <c r="Y5" s="35"/>
       <c r="Z5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA5" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
@@ -1932,7 +1935,7 @@
       <c r="AI5" s="29"/>
       <c r="AJ5" s="30"/>
       <c r="AK5" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AL5" s="45"/>
       <c r="AM5" s="45"/>
@@ -1940,7 +1943,7 @@
       <c r="AO5" s="45"/>
       <c r="AP5" s="47"/>
       <c r="AQ5" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AR5" s="25"/>
       <c r="AS5" s="25"/>
@@ -1949,12 +1952,12 @@
       <c r="AV5" s="25"/>
       <c r="AW5" s="25"/>
       <c r="AX5" s="25"/>
-      <c r="AY5" s="25"/>
-      <c r="AZ5" s="26"/>
+      <c r="AY5" s="26"/>
+      <c r="AZ5" s="50"/>
       <c r="BA5" s="18"/>
       <c r="BB5" s="18"/>
     </row>
-    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1971,13 +1974,13 @@
         <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>4</v>
@@ -1992,7 +1995,7 @@
         <v>24</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>7</v>
@@ -2016,7 +2019,7 @@
         <v>13</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>6</v>
@@ -2028,10 +2031,10 @@
         <v>3</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA6" s="2" t="s">
         <v>14</v>
@@ -2040,13 +2043,13 @@
         <v>15</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AF6" s="3" t="s">
         <v>17</v>
@@ -2055,13 +2058,13 @@
         <v>18</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AI6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AJ6" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AK6" s="3" t="s">
         <v>27</v>
@@ -2082,216 +2085,216 @@
         <v>72</v>
       </c>
       <c r="AQ6" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AR6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="AS6" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AT6" s="9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AU6" s="9" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="AV6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AW6" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="AX6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AZ6" s="8" t="s">
+      <c r="AY6" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="AZ6" s="49" t="s">
+        <v>73</v>
+      </c>
       <c r="BA6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BB6" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.2">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AQ5:AZ5"/>
+    <mergeCell ref="AQ5:AY5"/>
     <mergeCell ref="AA5:AJ5"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="W5:Y5"/>
@@ -2318,24 +2321,24 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.83203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2347,16 +2350,16 @@
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -2366,17 +2369,17 @@
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
       <c r="J3" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="35"/>
       <c r="L3" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M3" s="47"/>
     </row>
-    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
@@ -2388,19 +2391,19 @@
         <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
@@ -2412,178 +2415,178 @@
         <v>27</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2607,20 +2610,20 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2628,29 +2631,29 @@
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>59</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -2658,9 +2661,9 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>

</xml_diff>

<commit_message>
condo desk review (#135)
* condo desk review

* lintr
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1455155-E707-422A-AE82-4E35DDC6E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3991A33C-F26A-4683-BCC0-EBDF0F0957AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -565,21 +565,9 @@
     <t>Sale Num. Parcels 2</t>
   </si>
   <si>
-    <t>Average AV Difference</t>
-  </si>
-  <si>
     <t>Average YoY ∆ %</t>
   </si>
   <si>
-    <t>Max AV</t>
-  </si>
-  <si>
-    <t>Average AV</t>
-  </si>
-  <si>
-    <t>Min AV</t>
-  </si>
-  <si>
     <t>Sale Ratio</t>
   </si>
   <si>
@@ -593,6 +581,18 @@
   </si>
   <si>
     <t>Recent Assessable Permit</t>
+  </si>
+  <si>
+    <t>Min MV</t>
+  </si>
+  <si>
+    <t>Average MV</t>
+  </si>
+  <si>
+    <t>Max MV</t>
+  </si>
+  <si>
+    <t>Average MV Difference</t>
   </si>
 </sst>
 </file>
@@ -904,6 +904,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -977,12 +983,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,11 +1012,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean Cochrane" refreshedDate="45699.714398958335" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46063.730929745368" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
-  <cacheFields count="53">
+  <cacheFields count="54">
     <cacheField name="PIN" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
@@ -1170,6 +1170,9 @@
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="YoY Change &lt;= -5%" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Recent Assessable Permit" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="Total AV" numFmtId="0">
@@ -1243,6 +1246,7 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1250,10 +1254,10 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7822879B-2883-4C2B-8FC0-C7DD3997BA21}" name="Neighborhood Breakout" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="53">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+  <pivotFields count="54">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
@@ -1280,6 +1284,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1342,10 +1347,10 @@
     </i>
   </colItems>
   <dataFields count="5">
-    <dataField name="Min AV" fld="51" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV" fld="51" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Max AV" fld="51" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
-    <dataField name="Average AV Difference" fld="52" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Min MV" fld="52" subtotal="min" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average MV" fld="52" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Max MV" fld="52" subtotal="max" baseField="2" baseItem="0" numFmtId="164"/>
+    <dataField name="Average MV Difference" fld="53" subtotal="average" baseField="2" baseItem="0" numFmtId="164"/>
     <dataField name="Average YoY ∆ %" fld="23" subtotal="average" baseField="2" baseItem="0" numFmtId="165"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1659,67 +1664,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="AL7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AS6" sqref="AS6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.58203125" customWidth="1"/>
+    <col min="5" max="5" width="16.58203125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.08203125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.58203125" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.58203125" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.58203125" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.83203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.58203125" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.08203125" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.58203125" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.58203125" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
-    <col min="42" max="42" width="12.875" customWidth="1"/>
-    <col min="43" max="45" width="15.625" customWidth="1"/>
-    <col min="46" max="46" width="12.625" customWidth="1"/>
-    <col min="47" max="47" width="13.125" customWidth="1"/>
-    <col min="48" max="48" width="14.125" customWidth="1"/>
+    <col min="41" max="41" width="16.58203125" style="13" customWidth="1"/>
+    <col min="42" max="42" width="12.83203125" customWidth="1"/>
+    <col min="43" max="45" width="15.58203125" customWidth="1"/>
+    <col min="46" max="46" width="12.58203125" customWidth="1"/>
+    <col min="47" max="47" width="13.08203125" customWidth="1"/>
+    <col min="48" max="48" width="14.08203125" customWidth="1"/>
     <col min="50" max="51" width="14" customWidth="1"/>
     <col min="52" max="52" width="13" customWidth="1"/>
     <col min="53" max="53" width="7.75" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="9.375" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="15.125" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="15.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -1775,7 +1780,7 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1815,13 +1820,13 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1856,7 +1861,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1890,74 +1895,74 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="B5" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="33" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="35"/>
+      <c r="X5" s="36"/>
+      <c r="Y5" s="37"/>
       <c r="Z5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="AA5" s="27" t="s">
+      <c r="AA5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AB5" s="28"/>
-      <c r="AC5" s="28"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="28"/>
-      <c r="AG5" s="28"/>
-      <c r="AH5" s="28"/>
-      <c r="AI5" s="29"/>
-      <c r="AJ5" s="30"/>
-      <c r="AK5" s="44" t="s">
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="30"/>
+      <c r="AD5" s="31"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="31"/>
+      <c r="AJ5" s="32"/>
+      <c r="AK5" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="AL5" s="45"/>
-      <c r="AM5" s="45"/>
-      <c r="AN5" s="46"/>
-      <c r="AO5" s="45"/>
-      <c r="AP5" s="47"/>
-      <c r="AQ5" s="24" t="s">
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="48"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="49"/>
+      <c r="AQ5" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="25"/>
-      <c r="AU5" s="25"/>
-      <c r="AV5" s="25"/>
-      <c r="AW5" s="25"/>
-      <c r="AX5" s="25"/>
-      <c r="AY5" s="26"/>
-      <c r="AZ5" s="50"/>
+      <c r="AR5" s="27"/>
+      <c r="AS5" s="27"/>
+      <c r="AT5" s="27"/>
+      <c r="AU5" s="27"/>
+      <c r="AV5" s="27"/>
+      <c r="AW5" s="27"/>
+      <c r="AX5" s="27"/>
+      <c r="AY5" s="28"/>
+      <c r="AZ5" s="25"/>
       <c r="BA5" s="18"/>
       <c r="BB5" s="18"/>
     </row>
-    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2036,7 @@
         <v>3</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>53</v>
@@ -2079,13 +2084,13 @@
         <v>32</v>
       </c>
       <c r="AO6" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AP6" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AQ6" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AR6" s="9" t="s">
         <v>31</v>
@@ -2111,8 +2116,8 @@
       <c r="AY6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AZ6" s="49" t="s">
-        <v>73</v>
+      <c r="AZ6" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="BA6" s="2" t="s">
         <v>60</v>
@@ -2121,175 +2126,175 @@
         <v>61</v>
       </c>
     </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048519" s="13"/>
     </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048520" s="13"/>
     </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048521" s="13"/>
     </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048522" s="13"/>
     </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048523" s="13"/>
     </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048524" s="13"/>
     </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048525" s="13"/>
     </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048526" s="13"/>
     </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048527" s="13"/>
     </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048528" s="13"/>
     </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048529" s="13"/>
     </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048530" s="13"/>
     </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048531" s="13"/>
     </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048532" s="13"/>
     </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048533" s="13"/>
     </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048534" s="13"/>
     </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048535" s="13"/>
     </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048536" s="13"/>
     </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048537" s="13"/>
     </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048538" s="13"/>
     </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048539" s="13"/>
     </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048540" s="13"/>
     </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048541" s="13"/>
     </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048542" s="13"/>
     </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048543" s="13"/>
     </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048544" s="13"/>
     </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048545" s="13"/>
     </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048546" s="13"/>
     </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048547" s="13"/>
     </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048548" s="13"/>
     </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048549" s="13"/>
     </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048550" s="13"/>
     </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048551" s="13"/>
     </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048552" s="13"/>
     </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048553" s="13"/>
     </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048554" s="13"/>
     </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048555" s="13"/>
     </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048556" s="13"/>
     </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048557" s="13"/>
     </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048558" s="13"/>
     </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048559" s="13"/>
     </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048560" s="13"/>
     </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048561" s="13"/>
     </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048562" s="13"/>
     </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048563" s="13"/>
     </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048564" s="13"/>
     </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048565" s="13"/>
     </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048566" s="13"/>
     </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048567" s="13"/>
     </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048568" s="13"/>
     </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048569" s="13"/>
     </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048570" s="13"/>
     </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048571" s="13"/>
     </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048572" s="13"/>
     </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048573" s="13"/>
     </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048574" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048574" s="13"/>
     </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="38:38" x14ac:dyDescent="0.35">
       <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
@@ -2321,63 +2326,63 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="42.625" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.58203125" customWidth="1"/>
+    <col min="3" max="3" width="42.58203125" customWidth="1"/>
+    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="5" max="6" width="11.58203125" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.375" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.5">
+      <c r="B1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="17"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="44" t="s">
+      <c r="K3" s="37"/>
+      <c r="L3" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="47"/>
-    </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="M3" s="49"/>
+    </row>
+    <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -2418,175 +2423,175 @@
         <v>43</v>
       </c>
     </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048517" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048517" s="13"/>
     </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048518" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048518" s="13"/>
     </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048519" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048519" s="13"/>
     </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048520" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048520" s="13"/>
     </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048521" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048521" s="13"/>
     </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048522" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048522" s="13"/>
     </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048523" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048523" s="13"/>
     </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048524" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048524" s="13"/>
     </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048525" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048525" s="13"/>
     </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048526" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048526" s="13"/>
     </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048527" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048527" s="13"/>
     </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048528" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048528" s="13"/>
     </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048529" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048529" s="13"/>
     </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048530" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048530" s="13"/>
     </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048531" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048531" s="13"/>
     </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048532" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048532" s="13"/>
     </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048533" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048533" s="13"/>
     </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048534" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048534" s="13"/>
     </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048535" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048535" s="13"/>
     </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048536" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048536" s="13"/>
     </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048537" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048537" s="13"/>
     </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048538" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048538" s="13"/>
     </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048539" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048539" s="13"/>
     </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048540" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048540" s="13"/>
     </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048541" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048541" s="13"/>
     </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048542" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048542" s="13"/>
     </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048543" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048543" s="13"/>
     </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048544" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048544" s="13"/>
     </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048545" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048545" s="13"/>
     </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048546" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048546" s="13"/>
     </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048547" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048547" s="13"/>
     </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048548" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048548" s="13"/>
     </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048549" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048549" s="13"/>
     </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048550" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048550" s="13"/>
     </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048551" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048551" s="13"/>
     </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048552" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048552" s="13"/>
     </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048553" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048553" s="13"/>
     </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048554" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048554" s="13"/>
     </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048555" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048555" s="13"/>
     </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048556" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048556" s="13"/>
     </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048557" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048557" s="13"/>
     </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048558" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048558" s="13"/>
     </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048559" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048559" s="13"/>
     </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048560" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048560" s="13"/>
     </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048561" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048561" s="13"/>
     </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048562" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048562" s="13"/>
     </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048563" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048563" s="13"/>
     </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048564" s="13"/>
     </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048565" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048565" s="13"/>
     </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048566" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048566" s="13"/>
     </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048567" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048567" s="13"/>
     </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048568" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048568" s="13"/>
     </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048569" s="13"/>
     </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048570" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048570" s="13"/>
     </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048571" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048571" s="13"/>
     </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048572" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048572" s="13"/>
     </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="1048573" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M1048573" s="13"/>
     </row>
   </sheetData>
@@ -2606,52 +2611,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4264-9F60-48E3-A5EA-D04C0BA089E2}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="B1" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="F3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>58</v>
       </c>
@@ -2661,7 +2666,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
modify desk review template
</commit_message>
<xml_diff>
--- a/misc/desk_review_template.xlsx
+++ b/misc/desk_review_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3991A33C-F26A-4683-BCC0-EBDF0F0957AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8208B398-6B4C-4A12-9DB7-3262CEC5E1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIN Detail" sheetId="2" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46063.730929745368" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Damon Major" refreshedDate="46071.669750347224" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{71C4991D-10B4-4CFF-8A35-19A87D2DBFEA}">
   <cacheSource type="worksheet">
     <worksheetSource name="pin_detail_range"/>
   </cacheSource>
@@ -1662,60 +1662,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK1048575"/>
+  <dimension ref="A1:BK6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="AL7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AS6" sqref="AS6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="42.58203125" customWidth="1"/>
-    <col min="5" max="5" width="16.58203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="11" customWidth="1"/>
-    <col min="9" max="10" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="8" max="8" width="13.875" style="11" customWidth="1"/>
+    <col min="9" max="10" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="9.08203125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="13.58203125" style="15" customWidth="1"/>
-    <col min="16" max="17" width="11.58203125" style="10" customWidth="1"/>
-    <col min="18" max="18" width="13.58203125" style="10" customWidth="1"/>
+    <col min="12" max="13" width="10.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="15" customWidth="1"/>
+    <col min="16" max="17" width="11.625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="13.625" style="10" customWidth="1"/>
     <col min="19" max="19" width="11" style="10"/>
-    <col min="20" max="21" width="10.83203125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="11.58203125" style="11" customWidth="1"/>
+    <col min="20" max="21" width="10.875" style="10" customWidth="1"/>
+    <col min="22" max="22" width="11.625" style="11" customWidth="1"/>
     <col min="23" max="23" width="11" style="12"/>
     <col min="24" max="25" width="11" style="11"/>
-    <col min="26" max="26" width="21.08203125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.125" style="11" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="13" style="10" customWidth="1"/>
-    <col min="29" max="29" width="18.58203125" style="10" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="10" customWidth="1"/>
     <col min="30" max="32" width="13" style="16" customWidth="1"/>
     <col min="33" max="33" width="13" style="10" customWidth="1"/>
-    <col min="34" max="35" width="18.58203125" style="10" customWidth="1"/>
+    <col min="34" max="35" width="18.625" style="10" customWidth="1"/>
     <col min="36" max="36" width="13" style="16" customWidth="1"/>
     <col min="39" max="40" width="11" style="13"/>
-    <col min="41" max="41" width="16.58203125" style="13" customWidth="1"/>
-    <col min="42" max="42" width="12.83203125" customWidth="1"/>
-    <col min="43" max="45" width="15.58203125" customWidth="1"/>
-    <col min="46" max="46" width="12.58203125" customWidth="1"/>
-    <col min="47" max="47" width="13.08203125" customWidth="1"/>
-    <col min="48" max="48" width="14.08203125" customWidth="1"/>
+    <col min="41" max="41" width="16.625" style="13" customWidth="1"/>
+    <col min="42" max="42" width="12.875" customWidth="1"/>
+    <col min="43" max="45" width="15.625" customWidth="1"/>
+    <col min="46" max="46" width="12.625" customWidth="1"/>
+    <col min="47" max="47" width="13.125" customWidth="1"/>
+    <col min="48" max="48" width="14.125" customWidth="1"/>
     <col min="50" max="51" width="14" customWidth="1"/>
     <col min="52" max="52" width="13" customWidth="1"/>
     <col min="53" max="53" width="7.75" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="15.08203125" customWidth="1"/>
+    <col min="54" max="54" width="9.375" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:63" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1780,7 +1780,7 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1820,7 +1820,7 @@
       <c r="AN2"/>
       <c r="AO2"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="AN3"/>
       <c r="AO3"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -1895,7 +1895,7 @@
       <c r="AN4"/>
       <c r="AO4"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>48</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="BA5" s="18"/>
       <c r="BB5" s="18"/>
     </row>
-    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2125,177 +2125,6 @@
       <c r="BB6" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="1048519" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048573" s="13"/>
-    </row>
-    <row r="1048574" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048574" s="13"/>
-    </row>
-    <row r="1048575" spans="38:38" x14ac:dyDescent="0.35">
-      <c r="AL1048575" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2317,31 +2146,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1048573"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.58203125" customWidth="1"/>
-    <col min="3" max="3" width="42.58203125" customWidth="1"/>
-    <col min="4" max="4" width="16.58203125" customWidth="1"/>
-    <col min="5" max="6" width="11.58203125" customWidth="1"/>
-    <col min="7" max="7" width="12.58203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="26" style="10" customWidth="1"/>
-    <col min="9" max="9" width="31.83203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="31.875" style="11" customWidth="1"/>
     <col min="10" max="10" width="11" style="12"/>
     <col min="11" max="11" width="11" style="11"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="38" t="s">
         <v>44</v>
       </c>
@@ -2355,14 +2184,14 @@
       <c r="J1"/>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
@@ -2382,7 +2211,7 @@
       </c>
       <c r="M3" s="49"/>
     </row>
-    <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -2422,177 +2251,6 @@
       <c r="M4" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="1048517" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048517" s="13"/>
-    </row>
-    <row r="1048518" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048518" s="13"/>
-    </row>
-    <row r="1048519" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048519" s="13"/>
-    </row>
-    <row r="1048520" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048520" s="13"/>
-    </row>
-    <row r="1048521" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048521" s="13"/>
-    </row>
-    <row r="1048522" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048522" s="13"/>
-    </row>
-    <row r="1048523" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048523" s="13"/>
-    </row>
-    <row r="1048524" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048524" s="13"/>
-    </row>
-    <row r="1048525" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048525" s="13"/>
-    </row>
-    <row r="1048526" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048526" s="13"/>
-    </row>
-    <row r="1048527" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048527" s="13"/>
-    </row>
-    <row r="1048528" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048528" s="13"/>
-    </row>
-    <row r="1048529" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048529" s="13"/>
-    </row>
-    <row r="1048530" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048530" s="13"/>
-    </row>
-    <row r="1048531" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048531" s="13"/>
-    </row>
-    <row r="1048532" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048532" s="13"/>
-    </row>
-    <row r="1048533" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048533" s="13"/>
-    </row>
-    <row r="1048534" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048534" s="13"/>
-    </row>
-    <row r="1048535" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048535" s="13"/>
-    </row>
-    <row r="1048536" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048536" s="13"/>
-    </row>
-    <row r="1048537" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048537" s="13"/>
-    </row>
-    <row r="1048538" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048538" s="13"/>
-    </row>
-    <row r="1048539" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048539" s="13"/>
-    </row>
-    <row r="1048540" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048540" s="13"/>
-    </row>
-    <row r="1048541" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048541" s="13"/>
-    </row>
-    <row r="1048542" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048542" s="13"/>
-    </row>
-    <row r="1048543" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048543" s="13"/>
-    </row>
-    <row r="1048544" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048544" s="13"/>
-    </row>
-    <row r="1048545" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048545" s="13"/>
-    </row>
-    <row r="1048546" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048546" s="13"/>
-    </row>
-    <row r="1048547" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048547" s="13"/>
-    </row>
-    <row r="1048548" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048548" s="13"/>
-    </row>
-    <row r="1048549" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048549" s="13"/>
-    </row>
-    <row r="1048550" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048550" s="13"/>
-    </row>
-    <row r="1048551" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048551" s="13"/>
-    </row>
-    <row r="1048552" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048552" s="13"/>
-    </row>
-    <row r="1048553" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048553" s="13"/>
-    </row>
-    <row r="1048554" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048554" s="13"/>
-    </row>
-    <row r="1048555" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048555" s="13"/>
-    </row>
-    <row r="1048556" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048556" s="13"/>
-    </row>
-    <row r="1048557" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048557" s="13"/>
-    </row>
-    <row r="1048558" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048558" s="13"/>
-    </row>
-    <row r="1048559" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048559" s="13"/>
-    </row>
-    <row r="1048560" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048560" s="13"/>
-    </row>
-    <row r="1048561" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048561" s="13"/>
-    </row>
-    <row r="1048562" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048562" s="13"/>
-    </row>
-    <row r="1048563" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048563" s="13"/>
-    </row>
-    <row r="1048564" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048564" s="13"/>
-    </row>
-    <row r="1048565" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048565" s="13"/>
-    </row>
-    <row r="1048566" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048566" s="13"/>
-    </row>
-    <row r="1048567" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048567" s="13"/>
-    </row>
-    <row r="1048568" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048568" s="13"/>
-    </row>
-    <row r="1048569" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048569" s="13"/>
-    </row>
-    <row r="1048570" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048570" s="13"/>
-    </row>
-    <row r="1048571" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048571" s="13"/>
-    </row>
-    <row r="1048572" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048572" s="13"/>
-    </row>
-    <row r="1048573" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M1048573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2611,22 +2269,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4264-9F60-48E3-A5EA-D04C0BA089E2}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="38" t="s">
         <v>56</v>
       </c>
@@ -2636,7 +2294,7 @@
       <c r="F1" s="38"/>
       <c r="G1" s="38"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>57</v>
       </c>
@@ -2656,7 +2314,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>58</v>
       </c>
@@ -2666,7 +2324,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>59</v>
       </c>

</xml_diff>